<commit_message>
Dip tube trade study added
</commit_message>
<xml_diff>
--- a/ASME-BPV-SectionVIII-Calcs.xlsx
+++ b/ASME-BPV-SectionVIII-Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD Documents\Propulsion Github\Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BBB642-7538-4E12-A955-6F351E99AA27}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50306F1A-5AB9-403E-845B-8148BD3329B2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535" activeTab="2" xr2:uid="{838B0196-D158-479E-A7C6-911A07F6EFB7}"/>
   </bookViews>
@@ -26,8 +26,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dan</author>
+  </authors>
+  <commentList>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{54115B5C-47B3-4614-9055-2EA3E002CA64}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Makes sense because mass continuity, with Ullage taking into account density variations</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{9F188605-EE30-4C0D-A26D-BC3556D56C44}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Makes sense because mass continuity, with Ullage taking into account density variations</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>Inner Radius (in)</t>
   </si>
@@ -137,12 +195,6 @@
     <t>Worst Case Pressure Case Study</t>
   </si>
   <si>
-    <t>Volumetric Ullage % req to not vent  as temp rises to 75F (with only liq at 75F)</t>
-  </si>
-  <si>
-    <t>Height from top required</t>
-  </si>
-  <si>
     <t>Ullage Volume</t>
   </si>
   <si>
@@ -159,9 +211,6 @@
   </si>
   <si>
     <t>ft^3</t>
-  </si>
-  <si>
-    <t>Makes sense because mass continuity, with Ullage taking into account density variations</t>
   </si>
   <si>
     <t>Worst case internal tank pressure (located at bottom of RT) (psi)</t>
@@ -190,6 +239,93 @@
   <si>
     <t>&lt;</t>
   </si>
+  <si>
+    <t>MAX OP PRESSURES</t>
+  </si>
+  <si>
+    <t>Ullage Volume Required in shell</t>
+  </si>
+  <si>
+    <t>Height from top of storage volume required</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Volumetric Ullage % req to not vent  as temp rises to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>70F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (with only liq at</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 70F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Volumetric Ullage % req to not vent  as temp rises to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">75F </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(with only liq at </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>75F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -201,7 +337,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,13 +455,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -466,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -658,6 +813,18 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -668,9 +835,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -700,6 +864,9 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -709,17 +876,32 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3417,44 +3599,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="D5" s="79" t="s">
+      <c r="B5" s="83"/>
+      <c r="D5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="79"/>
+      <c r="E5" s="83"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3552,7 +3734,7 @@
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="61" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="62">
         <f>'N2O Pressure Calcs'!H53</f>
@@ -3563,7 +3745,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="59" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17" s="60">
         <f>B10*B16</f>
@@ -3581,7 +3763,7 @@
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="61" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B19" s="62">
         <f>'N2O Pressure Calcs'!J53</f>
@@ -3639,7 +3821,7 @@
   <dimension ref="A1:P819"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="I15" sqref="I15:I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3658,20 +3840,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="84"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="87"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
-      <c r="G1" s="88" t="s">
+      <c r="G1" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="90"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="93"/>
       <c r="K1" s="47"/>
       <c r="L1" t="s">
         <v>27</v>
@@ -3701,14 +3883,14 @@
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86" t="s">
+      <c r="H2" s="89"/>
+      <c r="I2" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="87"/>
+      <c r="J2" s="90"/>
       <c r="K2" s="46"/>
       <c r="L2" t="s">
         <v>15</v>
@@ -3830,7 +4012,7 @@
         <v>756.46634647363703</v>
       </c>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M5">
         <v>0.87815195180003003</v>
@@ -3868,7 +4050,7 @@
         <v>761.51016398466595</v>
       </c>
       <c r="L6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M6">
         <v>1.25</v>
@@ -3906,7 +4088,7 @@
         <v>766.60204828473297</v>
       </c>
       <c r="L7" s="43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M7" s="43">
         <f>M5*M6</f>
@@ -5361,43 +5543,45 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="70">
+      <c r="A53" s="98">
         <v>75</v>
       </c>
-      <c r="B53" s="71">
+      <c r="B53" s="99">
         <f>B52+(((B54-B52)/($A$54-$A$52))*($A$53-$A$52))</f>
         <v>799.74517236666668</v>
       </c>
-      <c r="C53" s="44">
+      <c r="C53" s="100">
         <f t="shared" ref="C53:D53" si="6">C52+(((C54-C52)/($A$54-$A$52))*($A$53-$A$52))</f>
         <v>1.4612000162666667</v>
       </c>
-      <c r="D53" s="45">
+      <c r="D53" s="101">
         <f t="shared" si="6"/>
         <v>0.35142632153493331</v>
       </c>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="41">
+      <c r="E53" s="102"/>
+      <c r="F53" s="102"/>
+      <c r="G53" s="103">
         <f>G52+(((G54-G52)/($A$54-$A$52))*($A$53-$A$52))</f>
         <v>177.3738140488434</v>
       </c>
-      <c r="H53" s="45">
+      <c r="H53" s="101">
         <f t="shared" ref="H53" si="7">H52+(((H54-H52)/($A$54-$A$52))*($A$53-$A$52))</f>
         <v>977.11898641550999</v>
       </c>
-      <c r="I53" s="41">
+      <c r="I53" s="103">
         <f t="shared" ref="I53" si="8">I52+(((I54-I52)/($A$54-$A$52))*($A$53-$A$52))</f>
         <v>70.57596078568001</v>
       </c>
-      <c r="J53" s="45">
+      <c r="J53" s="101">
         <f t="shared" ref="J53" si="9">J52+(((J54-J52)/($A$54-$A$52))*($A$53-$A$52))</f>
         <v>1047.69494720119</v>
       </c>
       <c r="K53" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="L53" s="43"/>
+      <c r="L53" s="43" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
@@ -8470,11 +8654,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA32C0C-ED9A-4805-89D4-96E4CF8ECC22}">
-  <dimension ref="A1:P819"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA32C0C-ED9A-4805-89D4-96E4CF8ECC22}">
+  <dimension ref="A1:W819"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8482,49 +8666,61 @@
     <col min="1" max="1" width="11.42578125" style="24"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="23"/>
-    <col min="5" max="5" width="4.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="64"/>
     <col min="6" max="6" width="25.5703125" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" style="49" customWidth="1"/>
-    <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="14" max="15" width="19.85546875" customWidth="1"/>
+    <col min="16" max="16" width="26" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" style="49" customWidth="1"/>
+    <col min="19" max="19" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="91" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="94" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="94"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="47"/>
-      <c r="L1" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="95" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="47"/>
+      <c r="S1" t="s">
         <v>27</v>
       </c>
-      <c r="M1">
+      <c r="T1">
         <v>1.5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="V1" t="s">
         <v>31</v>
       </c>
-      <c r="P1">
+      <c r="W1">
         <v>3.2490157499999999</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>19</v>
       </c>
@@ -8537,38 +8733,55 @@
       <c r="D2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="92"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="96"/>
       <c r="G2" s="54" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="95" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="97" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="96" t="s">
+      <c r="K2" s="17"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" s="78" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" t="s">
         <v>15</v>
       </c>
-      <c r="M2">
-        <f>P1+(2*P3)</f>
+      <c r="T2">
+        <f>W1+(2*W3)</f>
         <v>3.7698490833333334</v>
       </c>
-      <c r="O2" t="s">
+      <c r="V2" t="s">
         <v>32</v>
       </c>
-      <c r="P2">
+      <c r="W2">
         <v>3.125</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>17</v>
       </c>
@@ -8581,34 +8794,51 @@
       <c r="D3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="93"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="97"/>
       <c r="G3" s="66" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H3" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="68" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="48"/>
-      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="17"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="48"/>
+      <c r="S3" t="s">
         <v>14</v>
       </c>
-      <c r="M3">
+      <c r="T3">
         <v>32.200000000000003</v>
       </c>
-      <c r="O3" t="s">
+      <c r="V3" t="s">
         <v>33</v>
       </c>
-      <c r="P3">
-        <f>P2/12</f>
+      <c r="W3">
+        <f>W2/12</f>
         <v>0.26041666666666669</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>32</v>
       </c>
@@ -8621,26 +8851,51 @@
       <c r="D4" s="25">
         <v>0.16525852904319999</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="41">
-        <f t="shared" ref="F4:F35" si="0">($C$53-C4)/(D4-C4)</f>
-        <v>0.18736491688811011</v>
+        <f>($C$47-C4)/(D4-C4)</f>
+        <v>0.15895834986355586</v>
       </c>
       <c r="G4" s="69">
-        <f>$M$7/((C4*(1-F4))+(D4*F4))</f>
-        <v>0.75122497093492424</v>
+        <f>$T$7/((C4*(1-F4))+(D4*F4))</f>
+        <v>0.72863533976250439</v>
       </c>
       <c r="H4" s="53">
         <f>G4*F4</f>
+        <v>0.11582267126091907</v>
+      </c>
+      <c r="I4" s="53">
+        <f>H4-$M$55</f>
+        <v>7.8834322787596306E-2</v>
+      </c>
+      <c r="J4" s="25">
+        <f>IF(I4&gt;0, ('BPV Calcs'!$B$8/12)+(I4/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.63043898282165145</v>
+      </c>
+      <c r="K4" s="17"/>
+      <c r="L4" s="41">
+        <f t="shared" ref="L4:L35" si="0">($C$53-C4)/(D4-C4)</f>
+        <v>0.18736491688811011</v>
+      </c>
+      <c r="M4" s="69">
+        <f t="shared" ref="M4:M35" si="1">$T$7/((C4*(1-L4))+(D4*L4))</f>
+        <v>0.75122497093492424</v>
+      </c>
+      <c r="N4" s="53">
+        <f>M4*L4</f>
         <v>0.14075320424349502</v>
       </c>
-      <c r="I4" s="25">
-        <f>IF(H4&gt;$G$55, $G$58-(G4*(1-F4)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>1.0078713506575352</v>
-      </c>
-      <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O4" s="53">
+        <f>N4-$M$55</f>
+        <v>0.10376485577017228</v>
+      </c>
+      <c r="P4" s="25">
+        <f>IF(I4&gt;0, ('BPV Calcs'!$B$8/12)+(O4/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.7474546839908689</v>
+      </c>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <v>32.9</v>
       </c>
@@ -8653,32 +8908,57 @@
       <c r="D5" s="25">
         <v>0.16772615040639999</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="53"/>
       <c r="F5" s="41">
+        <f t="shared" ref="F5:F46" si="2">($C$47-C5)/(D5-C5)</f>
+        <v>0.15658283861487579</v>
+      </c>
+      <c r="G5" s="69">
+        <f>$T$7/((C5*(1-F5))+(D5*F5))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H5" s="53">
+        <f t="shared" ref="H5:H45" si="3">G5*F5</f>
+        <v>0.11409178981512741</v>
+      </c>
+      <c r="I5" s="53">
+        <f t="shared" ref="I5:I47" si="4">H5-$M$55</f>
+        <v>7.7103441341804663E-2</v>
+      </c>
+      <c r="J5" s="25">
+        <f>IF(I5&gt;0, ('BPV Calcs'!$B$8/12)+(I5/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.62231479605991424</v>
+      </c>
+      <c r="K5" s="17"/>
+      <c r="L5" s="41">
         <f t="shared" si="0"/>
         <v>0.18512214630827489</v>
       </c>
-      <c r="G5" s="69">
-        <f>$M$7/((C5*(1-F5))+(D5*F5))</f>
+      <c r="M5" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H5" s="53">
-        <f t="shared" ref="H5:H53" si="1">G5*F5</f>
+      <c r="N5" s="53">
+        <f t="shared" ref="N5:N53" si="5">M5*L5</f>
         <v>0.13906837897984459</v>
       </c>
-      <c r="I5" s="25">
-        <f>IF(H5&gt;$G$55, $G$58-(G5*(1-F5)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.99996333642809798</v>
-      </c>
-      <c r="J5" s="17"/>
-      <c r="L5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5">
+      <c r="O5" s="53">
+        <f t="shared" ref="O5:O53" si="6">N5-$M$55</f>
+        <v>0.10208003050652184</v>
+      </c>
+      <c r="P5" s="25">
+        <f>IF(I5&gt;0, ('BPV Calcs'!$B$8/12)+(O5/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.73954666976143157</v>
+      </c>
+      <c r="Q5" s="17"/>
+      <c r="S5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5">
         <v>0.87815195180003003</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>33.799999999999997</v>
       </c>
@@ -8691,32 +8971,57 @@
       <c r="D6" s="25">
         <v>0.1702317244288</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="53"/>
       <c r="F6" s="41">
+        <f t="shared" si="2"/>
+        <v>0.1541689886823846</v>
+      </c>
+      <c r="G6" s="69">
+        <f>$T$7/((C6*(1-F6))+(D6*F6))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H6" s="53">
+        <f t="shared" si="3"/>
+        <v>0.112332973449431</v>
+      </c>
+      <c r="I6" s="53">
+        <f t="shared" si="4"/>
+        <v>7.5344624976108249E-2</v>
+      </c>
+      <c r="J6" s="25">
+        <f>IF(I6&gt;0, ('BPV Calcs'!$B$8/12)+(I6/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.61405949199546828</v>
+      </c>
+      <c r="K6" s="17"/>
+      <c r="L6" s="41">
         <f t="shared" si="0"/>
         <v>0.18284364136366457</v>
       </c>
-      <c r="G6" s="69">
-        <f>$M$7/((C6*(1-F6))+(D6*F6))</f>
+      <c r="M6" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H6" s="53">
-        <f t="shared" si="1"/>
+      <c r="N6" s="53">
+        <f t="shared" si="5"/>
         <v>0.13735670916905462</v>
       </c>
-      <c r="I6" s="25">
-        <f>IF(H6&gt;$G$55, $G$58-(G6*(1-F6)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.99192932274617007</v>
-      </c>
-      <c r="J6" s="17"/>
-      <c r="L6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6">
+      <c r="O6" s="53">
+        <f t="shared" si="6"/>
+        <v>0.10036836069573188</v>
+      </c>
+      <c r="P6" s="25">
+        <f>IF(I6&gt;0, ('BPV Calcs'!$B$8/12)+(O6/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.73151265607950378</v>
+      </c>
+      <c r="Q6" s="17"/>
+      <c r="S6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6">
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>34.700000000000003</v>
       </c>
@@ -8729,33 +9034,58 @@
       <c r="D7" s="25">
         <v>0.17277604664159998</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="53"/>
       <c r="F7" s="41">
+        <f t="shared" si="2"/>
+        <v>0.15171807787171285</v>
+      </c>
+      <c r="G7" s="69">
+        <f>$T$7/((C7*(1-F7))+(D7*F7))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H7" s="53">
+        <f t="shared" si="3"/>
+        <v>0.11054715321816959</v>
+      </c>
+      <c r="I7" s="53">
+        <f t="shared" si="4"/>
+        <v>7.3558804744846829E-2</v>
+      </c>
+      <c r="J7" s="25">
+        <f>IF(I7&gt;0, ('BPV Calcs'!$B$8/12)+(I7/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.60567744069037677</v>
+      </c>
+      <c r="K7" s="17"/>
+      <c r="L7" s="41">
         <f t="shared" si="0"/>
         <v>0.18053067987595114</v>
       </c>
-      <c r="G7" s="69">
-        <f>$M$7/((C7*(1-F7))+(D7*F7))</f>
+      <c r="M7" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H7" s="53">
-        <f t="shared" si="1"/>
+      <c r="N7" s="53">
+        <f t="shared" si="5"/>
         <v>0.1356191547426735</v>
       </c>
-      <c r="I7" s="25">
-        <f>IF(H7&gt;$G$55, $G$58-(G7*(1-F7)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.98377381521390994</v>
-      </c>
-      <c r="J7" s="17"/>
-      <c r="L7" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="43">
-        <f>M5*M6</f>
+      <c r="O7" s="53">
+        <f t="shared" si="6"/>
+        <v>9.8630806269350751E-2</v>
+      </c>
+      <c r="P7" s="25">
+        <f>IF(I7&gt;0, ('BPV Calcs'!$B$8/12)+(O7/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.72335714854724331</v>
+      </c>
+      <c r="Q7" s="17"/>
+      <c r="S7" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7" s="43">
+        <f>T5*T6</f>
         <v>1.0976899397500375</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>35.6</v>
       </c>
@@ -8768,26 +9098,51 @@
       <c r="D8" s="25">
         <v>0.17536002899519998</v>
       </c>
-      <c r="E8" s="17"/>
+      <c r="E8" s="53"/>
       <c r="F8" s="41">
+        <f t="shared" si="2"/>
+        <v>0.14922826351373839</v>
+      </c>
+      <c r="G8" s="69">
+        <f>$T$7/((C8*(1-F8))+(D8*F8))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H8" s="53">
+        <f t="shared" si="3"/>
+        <v>0.10873298648750131</v>
+      </c>
+      <c r="I8" s="53">
+        <f t="shared" si="4"/>
+        <v>7.1744638014178547E-2</v>
+      </c>
+      <c r="J8" s="25">
+        <f>IF(I8&gt;0, ('BPV Calcs'!$B$8/12)+(I8/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.59716234026410897</v>
+      </c>
+      <c r="K8" s="17"/>
+      <c r="L8" s="41">
         <f t="shared" si="0"/>
         <v>0.17818152870115089</v>
       </c>
-      <c r="G8" s="69">
-        <f>$M$7/((C8*(1-F8))+(D8*F8))</f>
+      <c r="M8" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H8" s="53">
-        <f t="shared" si="1"/>
+      <c r="N8" s="53">
+        <f t="shared" si="5"/>
         <v>0.13385441371966245</v>
       </c>
-      <c r="I8" s="25">
-        <f>IF(H8&gt;$G$55, $G$58-(G8*(1-F8)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.97549070276163929</v>
-      </c>
-      <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O8" s="53">
+        <f t="shared" si="6"/>
+        <v>9.68660652463397E-2</v>
+      </c>
+      <c r="P8" s="25">
+        <f>IF(I8&gt;0, ('BPV Calcs'!$B$8/12)+(O8/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.71507403609497255</v>
+      </c>
+      <c r="Q8" s="17"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>36.5</v>
       </c>
@@ -8800,26 +9155,51 @@
       <c r="D9" s="25">
         <v>0.17798456403679999</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="53"/>
       <c r="F9" s="41">
+        <f t="shared" si="2"/>
+        <v>0.14669763583368992</v>
+      </c>
+      <c r="G9" s="69">
+        <f>$T$7/((C9*(1-F9))+(D9*F9))</f>
+        <v>0.72863533976250427</v>
+      </c>
+      <c r="H9" s="53">
+        <f t="shared" si="3"/>
+        <v>0.10688908172803678</v>
+      </c>
+      <c r="I9" s="53">
+        <f t="shared" si="4"/>
+        <v>6.990073325471402E-2</v>
+      </c>
+      <c r="J9" s="25">
+        <f>IF(I9&gt;0, ('BPV Calcs'!$B$8/12)+(I9/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.58850765933655724</v>
+      </c>
+      <c r="K9" s="17"/>
+      <c r="L9" s="41">
         <f t="shared" si="0"/>
         <v>0.17579439116722953</v>
       </c>
-      <c r="G9" s="69">
-        <f>$M$7/((C9*(1-F9))+(D9*F9))</f>
+      <c r="M9" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H9" s="53">
-        <f t="shared" si="1"/>
+      <c r="N9" s="53">
+        <f t="shared" si="5"/>
         <v>0.13206113639512471</v>
       </c>
-      <c r="I9" s="25">
-        <f>IF(H9&gt;$G$55, $G$58-(G9*(1-F9)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.96707365031962755</v>
-      </c>
-      <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O9" s="53">
+        <f t="shared" si="6"/>
+        <v>9.507278792180196E-2</v>
+      </c>
+      <c r="P9" s="25">
+        <f>IF(I9&gt;0, ('BPV Calcs'!$B$8/12)+(O9/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.70665698365296103</v>
+      </c>
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>37.4</v>
       </c>
@@ -8832,26 +9212,51 @@
       <c r="D10" s="25">
         <v>0.18065056371679999</v>
       </c>
-      <c r="E10" s="17"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="41">
+        <f t="shared" si="2"/>
+        <v>0.14412421839668005</v>
+      </c>
+      <c r="G10" s="69">
+        <f>$T$7/((C10*(1-F10))+(D10*F10))</f>
+        <v>0.72863533976250427</v>
+      </c>
+      <c r="H10" s="53">
+        <f t="shared" si="3"/>
+        <v>0.10501399883947034</v>
+      </c>
+      <c r="I10" s="53">
+        <f t="shared" si="4"/>
+        <v>6.8025650366147578E-2</v>
+      </c>
+      <c r="J10" s="25">
+        <f>IF(I10&gt;0, ('BPV Calcs'!$B$8/12)+(I10/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.57970663855174887</v>
+      </c>
+      <c r="K10" s="17"/>
+      <c r="L10" s="41">
         <f t="shared" si="0"/>
         <v>0.17336740843776965</v>
       </c>
-      <c r="G10" s="69">
-        <f>$M$7/((C10*(1-F10))+(D10*F10))</f>
+      <c r="M10" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H10" s="53">
-        <f t="shared" si="1"/>
+      <c r="N10" s="53">
+        <f t="shared" si="5"/>
         <v>0.13023792636472664</v>
       </c>
-      <c r="I10" s="25">
-        <f>IF(H10&gt;$G$55, $G$58-(G10*(1-F10)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.95851610362638651</v>
-      </c>
-      <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O10" s="53">
+        <f t="shared" si="6"/>
+        <v>9.3249577891403895E-2</v>
+      </c>
+      <c r="P10" s="25">
+        <f>IF(I10&gt;0, ('BPV Calcs'!$B$8/12)+(O10/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.69809943695971999</v>
+      </c>
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>38.299999999999997</v>
       </c>
@@ -8864,26 +9269,51 @@
       <c r="D11" s="25">
         <v>0.18335905640479999</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="53"/>
       <c r="F11" s="41">
+        <f t="shared" si="2"/>
+        <v>0.14150921576045203</v>
+      </c>
+      <c r="G11" s="69">
+        <f>$T$7/((C11*(1-F11))+(D11*F11))</f>
+        <v>0.7286353397625045</v>
+      </c>
+      <c r="H11" s="53">
+        <f t="shared" si="3"/>
+        <v>0.10310861550514253</v>
+      </c>
+      <c r="I11" s="53">
+        <f t="shared" si="4"/>
+        <v>6.6120267031819779E-2</v>
+      </c>
+      <c r="J11" s="25">
+        <f>IF(I11&gt;0, ('BPV Calcs'!$B$8/12)+(I11/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.57076339746587479</v>
+      </c>
+      <c r="K11" s="17"/>
+      <c r="L11" s="41">
         <f t="shared" si="0"/>
         <v>0.17090179823980461</v>
       </c>
-      <c r="G11" s="69">
-        <f>$M$7/((C11*(1-F11))+(D11*F11))</f>
+      <c r="M11" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492435</v>
       </c>
-      <c r="H11" s="53">
-        <f t="shared" si="1"/>
+      <c r="N11" s="53">
+        <f t="shared" si="5"/>
         <v>0.12838569841542352</v>
       </c>
-      <c r="I11" s="25">
-        <f>IF(H11&gt;$G$55, $G$58-(G11*(1-F11)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.94982235639023971</v>
-      </c>
-      <c r="J11" s="17"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O11" s="53">
+        <f t="shared" si="6"/>
+        <v>9.1397349942100775E-2</v>
+      </c>
+      <c r="P11" s="25">
+        <f>IF(I11&gt;0, ('BPV Calcs'!$B$8/12)+(O11/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.68940568972357363</v>
+      </c>
+      <c r="Q11" s="17"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>39.200000000000003</v>
       </c>
@@ -8896,26 +9326,51 @@
       <c r="D12" s="25">
         <v>0.18611099285759999</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="53"/>
       <c r="F12" s="41">
+        <f t="shared" si="2"/>
+        <v>0.13884731825649951</v>
+      </c>
+      <c r="G12" s="69">
+        <f>$T$7/((C12*(1-F12))+(D12*F12))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H12" s="53">
+        <f t="shared" si="3"/>
+        <v>0.1011690629129371</v>
+      </c>
+      <c r="I12" s="53">
+        <f t="shared" si="4"/>
+        <v>6.4180714439614345E-2</v>
+      </c>
+      <c r="J12" s="25">
+        <f>IF(I12&gt;0, ('BPV Calcs'!$B$8/12)+(I12/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.56165977715057258</v>
+      </c>
+      <c r="K12" s="17"/>
+      <c r="L12" s="41">
         <f t="shared" si="0"/>
         <v>0.16839248697229939</v>
       </c>
-      <c r="G12" s="69">
-        <f>$M$7/((C12*(1-F12))+(D12*F12))</f>
+      <c r="M12" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H12" s="53">
-        <f t="shared" si="1"/>
+      <c r="N12" s="53">
+        <f t="shared" si="5"/>
         <v>0.12650064113142523</v>
       </c>
-      <c r="I12" s="25">
-        <f>IF(H12&gt;$G$55, $G$58-(G12*(1-F12)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.94097451908225427</v>
-      </c>
-      <c r="J12" s="17"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O12" s="53">
+        <f t="shared" si="6"/>
+        <v>8.9512292658102482E-2</v>
+      </c>
+      <c r="P12" s="25">
+        <f>IF(I12&gt;0, ('BPV Calcs'!$B$8/12)+(O12/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.68055785241558797</v>
+      </c>
+      <c r="Q12" s="17"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <v>40.1</v>
       </c>
@@ -8928,26 +9383,51 @@
       <c r="D13" s="25">
         <v>0.1889074790576</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="53"/>
       <c r="F13" s="41">
+        <f t="shared" si="2"/>
+        <v>0.13614073631623833</v>
+      </c>
+      <c r="G13" s="69">
+        <f>$T$7/((C13*(1-F13))+(D13*F13))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H13" s="53">
+        <f t="shared" si="3"/>
+        <v>9.9196951661299826E-2</v>
+      </c>
+      <c r="I13" s="53">
+        <f t="shared" si="4"/>
+        <v>6.2208603187977073E-2</v>
+      </c>
+      <c r="J13" s="25">
+        <f>IF(I13&gt;0, ('BPV Calcs'!$B$8/12)+(I13/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.55240333722386414</v>
+      </c>
+      <c r="K13" s="17"/>
+      <c r="L13" s="41">
         <f t="shared" si="0"/>
         <v>0.16584166910419268</v>
       </c>
-      <c r="G13" s="69">
-        <f>$M$7/((C13*(1-F13))+(D13*F13))</f>
+      <c r="M13" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H13" s="53">
-        <f t="shared" si="1"/>
+      <c r="N13" s="53">
+        <f t="shared" si="5"/>
         <v>0.12458440305259647</v>
       </c>
-      <c r="I13" s="25">
-        <f>IF(H13&gt;$G$55, $G$58-(G13*(1-F13)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.93198032940496134</v>
-      </c>
-      <c r="J13" s="17"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O13" s="53">
+        <f t="shared" si="6"/>
+        <v>8.7596054579273719E-2</v>
+      </c>
+      <c r="P13" s="25">
+        <f>IF(I13&gt;0, ('BPV Calcs'!$B$8/12)+(O13/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.67156366273829482</v>
+      </c>
+      <c r="Q13" s="17"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <v>41</v>
       </c>
@@ -8960,26 +9440,51 @@
       <c r="D14" s="25">
         <v>0.19174958218079999</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="53"/>
       <c r="F14" s="41">
+        <f t="shared" si="2"/>
+        <v>0.1333850924260572</v>
+      </c>
+      <c r="G14" s="69">
+        <f>$T$7/((C14*(1-F14))+(D14*F14))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H14" s="53">
+        <f t="shared" si="3"/>
+        <v>9.718909213911324E-2</v>
+      </c>
+      <c r="I14" s="53">
+        <f t="shared" si="4"/>
+        <v>6.0200743665790486E-2</v>
+      </c>
+      <c r="J14" s="25">
+        <f>IF(I14&gt;0, ('BPV Calcs'!$B$8/12)+(I14/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.54297910670291372</v>
+      </c>
+      <c r="K14" s="17"/>
+      <c r="L14" s="41">
         <f t="shared" si="0"/>
         <v>0.16324517830239926</v>
       </c>
-      <c r="G14" s="69">
-        <f>$M$7/((C14*(1-F14))+(D14*F14))</f>
+      <c r="M14" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H14" s="53">
-        <f t="shared" si="1"/>
+      <c r="N14" s="53">
+        <f t="shared" si="5"/>
         <v>0.12263385432548642</v>
       </c>
-      <c r="I14" s="25">
-        <f>IF(H14&gt;$G$55, $G$58-(G14*(1-F14)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.9228250968583076</v>
-      </c>
-      <c r="J14" s="17"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O14" s="53">
+        <f t="shared" si="6"/>
+        <v>8.5645505852163656E-2</v>
+      </c>
+      <c r="P14" s="25">
+        <f>IF(I14&gt;0, ('BPV Calcs'!$B$8/12)+(O14/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.66240843019164086</v>
+      </c>
+      <c r="Q14" s="17"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <v>41.9</v>
       </c>
@@ -8992,26 +9497,51 @@
       <c r="D15" s="25">
         <v>0.19463846641919999</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E15" s="53"/>
       <c r="F15" s="41">
+        <f t="shared" si="2"/>
+        <v>0.13058032854768797</v>
+      </c>
+      <c r="G15" s="69">
+        <f>$T$7/((C15*(1-F15))+(D15*F15))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H15" s="53">
+        <f t="shared" si="3"/>
+        <v>9.5145442057644081E-2</v>
+      </c>
+      <c r="I15" s="53">
+        <f t="shared" si="4"/>
+        <v>5.8157093584321327E-2</v>
+      </c>
+      <c r="J15" s="25">
+        <f>IF(I15&gt;0, ('BPV Calcs'!$B$8/12)+(I15/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.5333868870983518</v>
+      </c>
+      <c r="K15" s="17"/>
+      <c r="L15" s="41">
         <f t="shared" si="0"/>
         <v>0.16060302380499611</v>
       </c>
-      <c r="G15" s="69">
-        <f>$M$7/((C15*(1-F15))+(D15*F15))</f>
+      <c r="M15" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H15" s="53">
-        <f t="shared" si="1"/>
+      <c r="N15" s="53">
+        <f t="shared" si="5"/>
         <v>0.12064900188996915</v>
       </c>
-      <c r="I15" s="25">
-        <f>IF(H15&gt;$G$55, $G$58-(G15*(1-F15)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.91350885401577342</v>
-      </c>
-      <c r="J15" s="17"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O15" s="53">
+        <f t="shared" si="6"/>
+        <v>8.3660653416646386E-2</v>
+      </c>
+      <c r="P15" s="25">
+        <f>IF(I15&gt;0, ('BPV Calcs'!$B$8/12)+(O15/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.65309218734910679</v>
+      </c>
+      <c r="Q15" s="17"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <v>42.8</v>
       </c>
@@ -9024,26 +9554,51 @@
       <c r="D16" s="25">
         <v>0.19757531536799999</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="53"/>
       <c r="F16" s="41">
+        <f t="shared" si="2"/>
+        <v>0.12772299193084816</v>
+      </c>
+      <c r="G16" s="69">
+        <f>$T$7/((C16*(1-F16))+(D16*F16))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H16" s="53">
+        <f t="shared" si="3"/>
+        <v>9.3063485621017156E-2</v>
+      </c>
+      <c r="I16" s="53">
+        <f t="shared" si="4"/>
+        <v>5.6075137147694402E-2</v>
+      </c>
+      <c r="J16" s="25">
+        <f>IF(I16&gt;0, ('BPV Calcs'!$B$8/12)+(I16/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.52361487009390451</v>
+      </c>
+      <c r="K16" s="17"/>
+      <c r="L16" s="41">
         <f t="shared" si="0"/>
         <v>0.15791193997714462</v>
       </c>
-      <c r="G16" s="69">
-        <f>$M$7/((C16*(1-F16))+(D16*F16))</f>
+      <c r="M16" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H16" s="53">
-        <f t="shared" si="1"/>
+      <c r="N16" s="53">
+        <f t="shared" si="5"/>
         <v>0.11862739251960797</v>
       </c>
-      <c r="I16" s="25">
-        <f>IF(H16&gt;$G$55, $G$58-(G16*(1-F16)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.90402008624139762</v>
-      </c>
-      <c r="J16" s="17"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O16" s="53">
+        <f t="shared" si="6"/>
+        <v>8.163904404628522E-2</v>
+      </c>
+      <c r="P16" s="25">
+        <f>IF(I16&gt;0, ('BPV Calcs'!$B$8/12)+(O16/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.64360341957473133</v>
+      </c>
+      <c r="Q16" s="17"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
         <v>43.7</v>
       </c>
@@ -9056,26 +9611,51 @@
       <c r="D17" s="25">
         <v>0.20056135142879999</v>
       </c>
-      <c r="E17" s="17"/>
+      <c r="E17" s="53"/>
       <c r="F17" s="41">
+        <f t="shared" si="2"/>
+        <v>0.1248117746228357</v>
+      </c>
+      <c r="G17" s="69">
+        <f>$T$7/((C17*(1-F17))+(D17*F17))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H17" s="53">
+        <f t="shared" si="3"/>
+        <v>9.0942269808671011E-2</v>
+      </c>
+      <c r="I17" s="53">
+        <f t="shared" si="4"/>
+        <v>5.3953921335348258E-2</v>
+      </c>
+      <c r="J17" s="25">
+        <f>IF(I17&gt;0, ('BPV Calcs'!$B$8/12)+(I17/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.51365858252530772</v>
+      </c>
+      <c r="K17" s="17"/>
+      <c r="L17" s="41">
         <f t="shared" si="0"/>
         <v>0.15517073555268265</v>
       </c>
-      <c r="G17" s="69">
-        <f>$M$7/((C17*(1-F17))+(D17*F17))</f>
+      <c r="M17" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492435</v>
       </c>
-      <c r="H17" s="53">
-        <f t="shared" si="1"/>
+      <c r="N17" s="53">
+        <f t="shared" si="5"/>
         <v>0.11656813130551485</v>
       </c>
-      <c r="I17" s="25">
-        <f>IF(H17&gt;$G$55, $G$58-(G17*(1-F17)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.89435459312794929</v>
-      </c>
-      <c r="J17" s="17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O17" s="53">
+        <f t="shared" si="6"/>
+        <v>7.9579782832192109E-2</v>
+      </c>
+      <c r="P17" s="25">
+        <f>IF(I17&gt;0, ('BPV Calcs'!$B$8/12)+(O17/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.63393792646128322</v>
+      </c>
+      <c r="Q17" s="17"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <v>44.6</v>
       </c>
@@ -9088,26 +9668,51 @@
       <c r="D18" s="25">
         <v>0.20359789401919998</v>
       </c>
-      <c r="E18" s="17"/>
+      <c r="E18" s="53"/>
       <c r="F18" s="41">
+        <f t="shared" si="2"/>
+        <v>0.12184531722222625</v>
+      </c>
+      <c r="G18" s="69">
+        <f>$T$7/((C18*(1-F18))+(D18*F18))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H18" s="53">
+        <f t="shared" si="3"/>
+        <v>8.8780804112686948E-2</v>
+      </c>
+      <c r="I18" s="53">
+        <f t="shared" si="4"/>
+        <v>5.1792455639364195E-2</v>
+      </c>
+      <c r="J18" s="25">
+        <f>IF(I18&gt;0, ('BPV Calcs'!$B$8/12)+(I18/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.50351337527500317</v>
+      </c>
+      <c r="K18" s="17"/>
+      <c r="L18" s="41">
         <f t="shared" si="0"/>
         <v>0.15237817442287846</v>
       </c>
-      <c r="G18" s="69">
-        <f>$M$7/((C18*(1-F18))+(D18*F18))</f>
+      <c r="M18" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H18" s="53">
-        <f t="shared" si="1"/>
+      <c r="N18" s="53">
+        <f t="shared" si="5"/>
         <v>0.11447028965194368</v>
       </c>
-      <c r="I18" s="25">
-        <f>IF(H18&gt;$G$55, $G$58-(G18*(1-F18)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.88450801615319419</v>
-      </c>
-      <c r="J18" s="17"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O18" s="53">
+        <f t="shared" si="6"/>
+        <v>7.7481941178620922E-2</v>
+      </c>
+      <c r="P18" s="25">
+        <f>IF(I18&gt;0, ('BPV Calcs'!$B$8/12)+(O18/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.62409134948652745</v>
+      </c>
+      <c r="Q18" s="17"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>45.5</v>
       </c>
@@ -9120,26 +9725,51 @@
       <c r="D19" s="25">
         <v>0.20668630136319999</v>
       </c>
-      <c r="E19" s="17"/>
+      <c r="E19" s="53"/>
       <c r="F19" s="41">
+        <f t="shared" si="2"/>
+        <v>0.11882104131137136</v>
+      </c>
+      <c r="G19" s="69">
+        <f>$T$7/((C19*(1-F19))+(D19*F19))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H19" s="53">
+        <f t="shared" si="3"/>
+        <v>8.6577209806845648E-2</v>
+      </c>
+      <c r="I19" s="53">
+        <f t="shared" si="4"/>
+        <v>4.9588861333522895E-2</v>
+      </c>
+      <c r="J19" s="25">
+        <f>IF(I19&gt;0, ('BPV Calcs'!$B$8/12)+(I19/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.493170430221613</v>
+      </c>
+      <c r="K19" s="17"/>
+      <c r="L19" s="41">
         <f t="shared" si="0"/>
         <v>0.14953184761109797</v>
       </c>
-      <c r="G19" s="69">
-        <f>$M$7/((C19*(1-F19))+(D19*F19))</f>
+      <c r="M19" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H19" s="53">
-        <f t="shared" si="1"/>
+      <c r="N19" s="53">
+        <f t="shared" si="5"/>
         <v>0.11233205787549259</v>
       </c>
-      <c r="I19" s="25">
-        <f>IF(H19&gt;$G$55, $G$58-(G19*(1-F19)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.87447186125997156</v>
-      </c>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O19" s="53">
+        <f t="shared" si="6"/>
+        <v>7.5343709402169834E-2</v>
+      </c>
+      <c r="P19" s="25">
+        <f>IF(I19&gt;0, ('BPV Calcs'!$B$8/12)+(O19/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.61405519459330482</v>
+      </c>
+      <c r="Q19" s="17"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>46.4</v>
       </c>
@@ -9152,26 +9782,51 @@
       <c r="D20" s="25">
         <v>0.2098279704912</v>
       </c>
-      <c r="E20" s="17"/>
+      <c r="E20" s="53"/>
       <c r="F20" s="41">
+        <f t="shared" si="2"/>
+        <v>0.11573626116593252</v>
+      </c>
+      <c r="G20" s="69">
+        <f>$T$7/((C20*(1-F20))+(D20*F20))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H20" s="53">
+        <f t="shared" si="3"/>
+        <v>8.4329529977481194E-2</v>
+      </c>
+      <c r="I20" s="53">
+        <f t="shared" si="4"/>
+        <v>4.734118150415844E-2</v>
+      </c>
+      <c r="J20" s="25">
+        <f>IF(I20&gt;0, ('BPV Calcs'!$B$8/12)+(I20/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.48262056225766659</v>
+      </c>
+      <c r="K20" s="17"/>
+      <c r="L20" s="41">
         <f t="shared" si="0"/>
         <v>0.14662924681830652</v>
       </c>
-      <c r="G20" s="69">
-        <f>$M$7/((C20*(1-F20))+(D20*F20))</f>
+      <c r="M20" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492435</v>
       </c>
-      <c r="H20" s="53">
-        <f t="shared" si="1"/>
+      <c r="N20" s="53">
+        <f t="shared" si="5"/>
         <v>0.11015155167929216</v>
       </c>
-      <c r="I20" s="25">
-        <f>IF(H20&gt;$G$55, $G$58-(G20*(1-F20)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.86423728418010937</v>
-      </c>
-      <c r="J20" s="17"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O20" s="53">
+        <f t="shared" si="6"/>
+        <v>7.3163203205969418E-2</v>
+      </c>
+      <c r="P20" s="25">
+        <f>IF(I20&gt;0, ('BPV Calcs'!$B$8/12)+(O20/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.60382061751344285</v>
+      </c>
+      <c r="Q20" s="17"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <v>47.3</v>
       </c>
@@ -9184,26 +9839,51 @@
       <c r="D21" s="25">
         <v>0.21302437604639998</v>
       </c>
-      <c r="E21" s="17"/>
+      <c r="E21" s="53"/>
       <c r="F21" s="41">
+        <f t="shared" si="2"/>
+        <v>0.11258936129657487</v>
+      </c>
+      <c r="G21" s="69">
+        <f>$T$7/((C21*(1-F21))+(D21*F21))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H21" s="53">
+        <f t="shared" si="3"/>
+        <v>8.2036587521973195E-2</v>
+      </c>
+      <c r="I21" s="53">
+        <f t="shared" si="4"/>
+        <v>4.5048239048650442E-2</v>
+      </c>
+      <c r="J21" s="25">
+        <f>IF(I21&gt;0, ('BPV Calcs'!$B$8/12)+(I21/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.47185824645160424</v>
+      </c>
+      <c r="K21" s="17"/>
+      <c r="L21" s="41">
         <f t="shared" si="0"/>
         <v>0.14366890189539364</v>
       </c>
-      <c r="G21" s="69">
-        <f>$M$7/((C21*(1-F21))+(D21*F21))</f>
+      <c r="M21" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H21" s="53">
-        <f t="shared" si="1"/>
+      <c r="N21" s="53">
+        <f t="shared" si="5"/>
         <v>0.10792766665061956</v>
       </c>
-      <c r="I21" s="25">
-        <f>IF(H21&gt;$G$55, $G$58-(G21*(1-F21)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.85379910116445856</v>
-      </c>
-      <c r="J21" s="17"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O21" s="53">
+        <f t="shared" si="6"/>
+        <v>7.0939318177296817E-2</v>
+      </c>
+      <c r="P21" s="25">
+        <f>IF(I21&gt;0, ('BPV Calcs'!$B$8/12)+(O21/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.59338243449779193</v>
+      </c>
+      <c r="Q21" s="17"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <v>48.2</v>
       </c>
@@ -9216,26 +9896,51 @@
       <c r="D22" s="25">
         <v>0.21627710909119999</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="53"/>
       <c r="F22" s="41">
+        <f t="shared" si="2"/>
+        <v>0.10937627096550176</v>
+      </c>
+      <c r="G22" s="69">
+        <f>$T$7/((C22*(1-F22))+(D22*F22))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H22" s="53">
+        <f t="shared" si="3"/>
+        <v>7.9695416356904122E-2</v>
+      </c>
+      <c r="I22" s="53">
+        <f t="shared" si="4"/>
+        <v>4.2707067883581369E-2</v>
+      </c>
+      <c r="J22" s="25">
+        <f>IF(I22&gt;0, ('BPV Calcs'!$B$8/12)+(I22/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.46086956098590726</v>
+      </c>
+      <c r="K22" s="17"/>
+      <c r="L22" s="41">
         <f t="shared" si="0"/>
         <v>0.14064697985759764</v>
       </c>
-      <c r="G22" s="69">
-        <f>$M$7/((C22*(1-F22))+(D22*F22))</f>
+      <c r="M22" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H22" s="53">
-        <f t="shared" si="1"/>
+      <c r="N22" s="53">
+        <f t="shared" si="5"/>
         <v>0.10565752335560866</v>
       </c>
-      <c r="I22" s="25">
-        <f>IF(H22&gt;$G$55, $G$58-(G22*(1-F22)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.84314379709992204</v>
-      </c>
-      <c r="J22" s="17"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O22" s="53">
+        <f t="shared" si="6"/>
+        <v>6.866917488228591E-2</v>
+      </c>
+      <c r="P22" s="25">
+        <f>IF(I22&gt;0, ('BPV Calcs'!$B$8/12)+(O22/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.58272713043325564</v>
+      </c>
+      <c r="Q22" s="17"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <v>49.1</v>
       </c>
@@ -9248,26 +9953,51 @@
       <c r="D23" s="25">
         <v>0.21958774128479999</v>
       </c>
-      <c r="E23" s="17"/>
+      <c r="E23" s="53"/>
       <c r="F23" s="41">
+        <f t="shared" si="2"/>
+        <v>0.10609514903040819</v>
+      </c>
+      <c r="G23" s="69">
+        <f>$T$7/((C23*(1-F23))+(D23*F23))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H23" s="53">
+        <f t="shared" si="3"/>
+        <v>7.730467496092501E-2</v>
+      </c>
+      <c r="I23" s="53">
+        <f t="shared" si="4"/>
+        <v>4.0316326487602257E-2</v>
+      </c>
+      <c r="J23" s="25">
+        <f>IF(I23&gt;0, ('BPV Calcs'!$B$8/12)+(I23/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.44964820920171994</v>
+      </c>
+      <c r="K23" s="17"/>
+      <c r="L23" s="41">
         <f t="shared" si="0"/>
         <v>0.13756180288548553</v>
       </c>
-      <c r="G23" s="69">
-        <f>$M$7/((C23*(1-F23))+(D23*F23))</f>
+      <c r="M23" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492413</v>
       </c>
-      <c r="H23" s="53">
-        <f t="shared" si="1"/>
+      <c r="N23" s="53">
+        <f t="shared" si="5"/>
         <v>0.10333986137440462</v>
       </c>
-      <c r="I23" s="25">
-        <f>IF(H23&gt;$G$55, $G$58-(G23*(1-F23)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.83226545599131585</v>
-      </c>
-      <c r="J23" s="17"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O23" s="53">
+        <f t="shared" si="6"/>
+        <v>6.6351512901081877E-2</v>
+      </c>
+      <c r="P23" s="25">
+        <f>IF(I23&gt;0, ('BPV Calcs'!$B$8/12)+(O23/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.57184878932464911</v>
+      </c>
+      <c r="Q23" s="17"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
         <v>50</v>
       </c>
@@ -9280,26 +10010,51 @@
       <c r="D24" s="25">
         <v>0.22295801891519998</v>
       </c>
-      <c r="E24" s="17"/>
+      <c r="E24" s="53"/>
       <c r="F24" s="41">
+        <f t="shared" si="2"/>
+        <v>0.10274285797407841</v>
+      </c>
+      <c r="G24" s="69">
+        <f>$T$7/((C24*(1-F24))+(D24*F24))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H24" s="53">
+        <f t="shared" si="3"/>
+        <v>7.4862077228113361E-2</v>
+      </c>
+      <c r="I24" s="53">
+        <f t="shared" si="4"/>
+        <v>3.7873728754790607E-2</v>
+      </c>
+      <c r="J24" s="25">
+        <f>IF(I24&gt;0, ('BPV Calcs'!$B$8/12)+(I24/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.43818346087166787</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="41">
         <f t="shared" si="0"/>
         <v>0.13441045075864813</v>
       </c>
-      <c r="G24" s="69">
-        <f>$M$7/((C24*(1-F24))+(D24*F24))</f>
+      <c r="M24" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H24" s="53">
-        <f t="shared" si="1"/>
+      <c r="N24" s="53">
+        <f t="shared" si="5"/>
         <v>0.10097248696451551</v>
       </c>
-      <c r="I24" s="25">
-        <f>IF(H24&gt;$G$55, $G$58-(G24*(1-F24)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.8211537811347509</v>
-      </c>
-      <c r="J24" s="17"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O24" s="53">
+        <f t="shared" si="6"/>
+        <v>6.3984138491192749E-2</v>
+      </c>
+      <c r="P24" s="25">
+        <f>IF(I24&gt;0, ('BPV Calcs'!$B$8/12)+(O24/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.56073711446808461</v>
+      </c>
+      <c r="Q24" s="17"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
         <v>50.9</v>
       </c>
@@ -9312,26 +10067,51 @@
       <c r="D25" s="25">
         <v>0.22638970767359998</v>
       </c>
-      <c r="E25" s="17"/>
+      <c r="E25" s="53"/>
       <c r="F25" s="41">
+        <f t="shared" si="2"/>
+        <v>9.9317342419351473E-2</v>
+      </c>
+      <c r="G25" s="69">
+        <f>$T$7/((C25*(1-F25))+(D25*F25))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H25" s="53">
+        <f t="shared" si="3"/>
+        <v>7.2366125538033149E-2</v>
+      </c>
+      <c r="I25" s="53">
+        <f t="shared" si="4"/>
+        <v>3.5377777064710396E-2</v>
+      </c>
+      <c r="J25" s="25">
+        <f>IF(I25&gt;0, ('BPV Calcs'!$B$8/12)+(I25/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.42646828665925313</v>
+      </c>
+      <c r="K25" s="17"/>
+      <c r="L25" s="41">
         <f t="shared" si="0"/>
         <v>0.13119105233236464</v>
       </c>
-      <c r="G25" s="69">
-        <f>$M$7/((C25*(1-F25))+(D25*F25))</f>
+      <c r="M25" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H25" s="53">
-        <f t="shared" si="1"/>
+      <c r="N25" s="53">
+        <f t="shared" si="5"/>
         <v>9.8553994475302747E-2</v>
       </c>
-      <c r="I25" s="25">
-        <f>IF(H25&gt;$G$55, $G$58-(G25*(1-F25)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.80980217486963424</v>
-      </c>
-      <c r="J25" s="17"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O25" s="53">
+        <f t="shared" si="6"/>
+        <v>6.1565646001979994E-2</v>
+      </c>
+      <c r="P25" s="25">
+        <f>IF(I25&gt;0, ('BPV Calcs'!$B$8/12)+(O25/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.54938550820296761</v>
+      </c>
+      <c r="Q25" s="17"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
         <v>51.8</v>
       </c>
@@ -9344,26 +10124,51 @@
       <c r="D26" s="25">
         <v>0.22988470907359998</v>
       </c>
-      <c r="E26" s="17"/>
+      <c r="E26" s="53"/>
       <c r="F26" s="41">
+        <f t="shared" si="2"/>
+        <v>9.5813964526532028E-2</v>
+      </c>
+      <c r="G26" s="69">
+        <f>$T$7/((C26*(1-F26))+(D26*F26))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H26" s="53">
+        <f t="shared" si="3"/>
+        <v>6.9813440596782211E-2</v>
+      </c>
+      <c r="I26" s="53">
+        <f t="shared" si="4"/>
+        <v>3.2825092123459458E-2</v>
+      </c>
+      <c r="J26" s="25">
+        <f>IF(I26&gt;0, ('BPV Calcs'!$B$8/12)+(I26/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.41448682527319503</v>
+      </c>
+      <c r="K26" s="17"/>
+      <c r="L26" s="41">
         <f t="shared" si="0"/>
         <v>0.12789925363670013</v>
       </c>
-      <c r="G26" s="69">
-        <f>$M$7/((C26*(1-F26))+(D26*F26))</f>
+      <c r="M26" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492413</v>
       </c>
-      <c r="H26" s="53">
-        <f t="shared" si="1"/>
+      <c r="N26" s="53">
+        <f t="shared" si="5"/>
         <v>9.6081113095828549E-2</v>
       </c>
-      <c r="I26" s="25">
-        <f>IF(H26&gt;$G$55, $G$58-(G26*(1-F26)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.79819528508794724</v>
-      </c>
-      <c r="J26" s="17"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O26" s="53">
+        <f t="shared" si="6"/>
+        <v>5.9092764622505796E-2</v>
+      </c>
+      <c r="P26" s="25">
+        <f>IF(I26&gt;0, ('BPV Calcs'!$B$8/12)+(O26/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.5377786184212805</v>
+      </c>
+      <c r="Q26" s="17"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
         <v>52.7</v>
       </c>
@@ -9376,26 +10181,51 @@
       <c r="D27" s="25">
         <v>0.23344498283839998</v>
       </c>
-      <c r="E27" s="17"/>
+      <c r="E27" s="53"/>
       <c r="F27" s="41">
+        <f t="shared" si="2"/>
+        <v>9.2229125421012484E-2</v>
+      </c>
+      <c r="G27" s="69">
+        <f>$T$7/((C27*(1-F27))+(D27*F27))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H27" s="53">
+        <f t="shared" si="3"/>
+        <v>6.7201400137138059E-2</v>
+      </c>
+      <c r="I27" s="53">
+        <f t="shared" si="4"/>
+        <v>3.0213051663815306E-2</v>
+      </c>
+      <c r="J27" s="25">
+        <f>IF(I27&gt;0, ('BPV Calcs'!$B$8/12)+(I27/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.40222676865582369</v>
+      </c>
+      <c r="K27" s="17"/>
+      <c r="L27" s="41">
         <f t="shared" si="0"/>
         <v>0.12453171014032675</v>
       </c>
-      <c r="G27" s="69">
-        <f>$M$7/((C27*(1-F27))+(D27*F27))</f>
+      <c r="M27" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492413</v>
       </c>
-      <c r="H27" s="53">
-        <f t="shared" si="1"/>
+      <c r="N27" s="53">
+        <f t="shared" si="5"/>
         <v>9.3551330330643362E-2</v>
       </c>
-      <c r="I27" s="25">
-        <f>IF(H27&gt;$G$55, $G$58-(G27*(1-F27)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.78632131896452595</v>
-      </c>
-      <c r="J27" s="17"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O27" s="53">
+        <f t="shared" si="6"/>
+        <v>5.6562981857320609E-2</v>
+      </c>
+      <c r="P27" s="25">
+        <f>IF(I27&gt;0, ('BPV Calcs'!$B$8/12)+(O27/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.5259046522978591</v>
+      </c>
+      <c r="Q27" s="17"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
         <v>53.6</v>
       </c>
@@ -9408,26 +10238,51 @@
       <c r="D28" s="25">
         <v>0.23707262451360001</v>
       </c>
-      <c r="E28" s="17"/>
+      <c r="E28" s="53"/>
       <c r="F28" s="41">
+        <f t="shared" si="2"/>
+        <v>8.8560323374262145E-2</v>
+      </c>
+      <c r="G28" s="69">
+        <f>$T$7/((C28*(1-F28))+(D28*F28))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H28" s="53">
+        <f t="shared" si="3"/>
+        <v>6.4528181311282753E-2</v>
+      </c>
+      <c r="I28" s="53">
+        <f t="shared" si="4"/>
+        <v>2.753983283796E-2</v>
+      </c>
+      <c r="J28" s="25">
+        <f>IF(I28&gt;0, ('BPV Calcs'!$B$8/12)+(I28/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.38967956096055162</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="41">
         <f t="shared" si="0"/>
         <v>0.12108614470086151</v>
       </c>
-      <c r="G28" s="69">
-        <f>$M$7/((C28*(1-F28))+(D28*F28))</f>
+      <c r="M28" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H28" s="53">
-        <f t="shared" si="1"/>
+      <c r="N28" s="53">
+        <f t="shared" si="5"/>
         <v>9.0962935533526718E-2</v>
       </c>
-      <c r="I28" s="25">
-        <f>IF(H28&gt;$G$55, $G$58-(G28*(1-F28)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.7741722472900836</v>
-      </c>
-      <c r="J28" s="17"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O28" s="53">
+        <f t="shared" si="6"/>
+        <v>5.3974587060203964E-2</v>
+      </c>
+      <c r="P28" s="25">
+        <f>IF(I28&gt;0, ('BPV Calcs'!$B$8/12)+(O28/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.51375558062341697</v>
+      </c>
+      <c r="Q28" s="17"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
         <v>54.5</v>
       </c>
@@ -9440,26 +10295,51 @@
       <c r="D29" s="25">
         <v>0.2407698072576</v>
       </c>
-      <c r="E29" s="17"/>
+      <c r="E29" s="53"/>
       <c r="F29" s="41">
+        <f t="shared" si="2"/>
+        <v>8.4801071831599392E-2</v>
+      </c>
+      <c r="G29" s="69">
+        <f>$T$7/((C29*(1-F29))+(D29*F29))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H29" s="53">
+        <f t="shared" si="3"/>
+        <v>6.1789057786241962E-2</v>
+      </c>
+      <c r="I29" s="53">
+        <f t="shared" si="4"/>
+        <v>2.4800709312919209E-2</v>
+      </c>
+      <c r="J29" s="25">
+        <f>IF(I29&gt;0, ('BPV Calcs'!$B$8/12)+(I29/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.37682301833886922</v>
+      </c>
+      <c r="K29" s="17"/>
+      <c r="L29" s="41">
         <f t="shared" si="0"/>
         <v>0.11755644588442445</v>
       </c>
-      <c r="G29" s="69">
-        <f>$M$7/((C29*(1-F29))+(D29*F29))</f>
+      <c r="M29" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H29" s="53">
-        <f t="shared" si="1"/>
+      <c r="N29" s="53">
+        <f t="shared" si="5"/>
         <v>8.8311337642739754E-2</v>
       </c>
-      <c r="I29" s="25">
-        <f>IF(H29&gt;$G$55, $G$58-(G29*(1-F29)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.76172652113468597</v>
-      </c>
-      <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O29" s="53">
+        <f t="shared" si="6"/>
+        <v>5.1322989169417001E-2</v>
+      </c>
+      <c r="P29" s="25">
+        <f>IF(I29&gt;0, ('BPV Calcs'!$B$8/12)+(O29/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.50130985446801912</v>
+      </c>
+      <c r="Q29" s="17"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
         <v>55.4</v>
       </c>
@@ -9472,26 +10352,51 @@
       <c r="D30" s="25">
         <v>0.24453885945439999</v>
       </c>
-      <c r="E30" s="17"/>
+      <c r="E30" s="53"/>
       <c r="F30" s="41">
+        <f t="shared" si="2"/>
+        <v>8.0949764895709625E-2</v>
+      </c>
+      <c r="G30" s="69">
+        <f>$T$7/((C30*(1-F30))+(D30*F30))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H30" s="53">
+        <f t="shared" si="3"/>
+        <v>5.8982859448480231E-2</v>
+      </c>
+      <c r="I30" s="53">
+        <f t="shared" si="4"/>
+        <v>2.1994510975157477E-2</v>
+      </c>
+      <c r="J30" s="25">
+        <f>IF(I30&gt;0, ('BPV Calcs'!$B$8/12)+(I30/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.36365164866367694</v>
+      </c>
+      <c r="K30" s="17"/>
+      <c r="L30" s="41">
         <f t="shared" si="0"/>
         <v>0.11394121977368245</v>
       </c>
-      <c r="G30" s="69">
-        <f>$M$7/((C30*(1-F30))+(D30*F30))</f>
+      <c r="M30" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H30" s="53">
-        <f t="shared" si="1"/>
+      <c r="N30" s="53">
+        <f t="shared" si="5"/>
         <v>8.5595489512774417E-2</v>
       </c>
-      <c r="I30" s="25">
-        <f>IF(H30&gt;$G$55, $G$58-(G30*(1-F30)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.74897922554260532</v>
-      </c>
-      <c r="J30" s="17"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O30" s="53">
+        <f t="shared" si="6"/>
+        <v>4.8607141039451664E-2</v>
+      </c>
+      <c r="P30" s="25">
+        <f>IF(I30&gt;0, ('BPV Calcs'!$B$8/12)+(O30/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.48856255887593891</v>
+      </c>
+      <c r="Q30" s="17"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
         <v>56.3</v>
       </c>
@@ -9504,26 +10409,51 @@
       <c r="D31" s="25">
         <v>0.24838222590720002</v>
       </c>
-      <c r="E31" s="17"/>
+      <c r="E31" s="53"/>
       <c r="F31" s="41">
+        <f t="shared" si="2"/>
+        <v>7.7000755915053343E-2</v>
+      </c>
+      <c r="G31" s="69">
+        <f>$T$7/((C31*(1-F31))+(D31*F31))</f>
+        <v>0.7286353397625045</v>
+      </c>
+      <c r="H31" s="53">
+        <f t="shared" si="3"/>
+        <v>5.6105471948134568E-2</v>
+      </c>
+      <c r="I31" s="53">
+        <f t="shared" si="4"/>
+        <v>1.9117123474811815E-2</v>
+      </c>
+      <c r="J31" s="25">
+        <f>IF(I31&gt;0, ('BPV Calcs'!$B$8/12)+(I31/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.3501461405333931</v>
+      </c>
+      <c r="K31" s="17"/>
+      <c r="L31" s="41">
         <f t="shared" si="0"/>
         <v>0.11023518674553594</v>
       </c>
-      <c r="G31" s="69">
-        <f>$M$7/((C31*(1-F31))+(D31*F31))</f>
+      <c r="M31" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492413</v>
       </c>
-      <c r="H31" s="53">
-        <f t="shared" si="1"/>
+      <c r="N31" s="53">
+        <f t="shared" si="5"/>
         <v>8.2811424958921173E-2</v>
       </c>
-      <c r="I31" s="25">
-        <f>IF(H31&gt;$G$55, $G$58-(G31*(1-F31)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.73591174455063557</v>
-      </c>
-      <c r="J31" s="17"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O31" s="53">
+        <f t="shared" si="6"/>
+        <v>4.582307648559842E-2</v>
+      </c>
+      <c r="P31" s="25">
+        <f>IF(I31&gt;0, ('BPV Calcs'!$B$8/12)+(O31/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.4754950778839685</v>
+      </c>
+      <c r="Q31" s="17"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
         <v>57.2</v>
       </c>
@@ -9536,26 +10466,51 @@
       <c r="D32" s="25">
         <v>0.25230250664479997</v>
       </c>
-      <c r="E32" s="17"/>
+      <c r="E32" s="53"/>
       <c r="F32" s="41">
+        <f t="shared" si="2"/>
+        <v>7.2949435155999456E-2</v>
+      </c>
+      <c r="G32" s="69">
+        <f>$T$7/((C32*(1-F32))+(D32*F32))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H32" s="53">
+        <f t="shared" si="3"/>
+        <v>5.3153536470374449E-2</v>
+      </c>
+      <c r="I32" s="53">
+        <f t="shared" si="4"/>
+        <v>1.6165187997051696E-2</v>
+      </c>
+      <c r="J32" s="25">
+        <f>IF(I32&gt;0, ('BPV Calcs'!$B$8/12)+(I32/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.33629072877874644</v>
+      </c>
+      <c r="K32" s="17"/>
+      <c r="L32" s="41">
         <f t="shared" si="0"/>
         <v>0.10643407956180023</v>
       </c>
-      <c r="G32" s="69">
-        <f>$M$7/((C32*(1-F32))+(D32*F32))</f>
+      <c r="M32" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H32" s="53">
-        <f t="shared" si="1"/>
+      <c r="N32" s="53">
+        <f t="shared" si="5"/>
         <v>7.9955938325298792E-2</v>
       </c>
-      <c r="I32" s="25">
-        <f>IF(H32&gt;$G$55, $G$58-(G32*(1-F32)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.72250903186710858</v>
-      </c>
-      <c r="J32" s="17"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O32" s="53">
+        <f t="shared" si="6"/>
+        <v>4.2967589851976039E-2</v>
+      </c>
+      <c r="P32" s="25">
+        <f>IF(I32&gt;0, ('BPV Calcs'!$B$8/12)+(O32/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.46209236520044183</v>
+      </c>
+      <c r="Q32" s="17"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
         <v>58.1</v>
       </c>
@@ -9568,26 +10523,51 @@
       <c r="D33" s="25">
         <v>0.25630243751839998</v>
       </c>
-      <c r="E33" s="17"/>
+      <c r="E33" s="53"/>
       <c r="F33" s="41">
+        <f t="shared" si="2"/>
+        <v>6.8789593883226779E-2</v>
+      </c>
+      <c r="G33" s="69">
+        <f>$T$7/((C33*(1-F33))+(D33*F33))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H33" s="53">
+        <f t="shared" si="3"/>
+        <v>5.0122529111229636E-2</v>
+      </c>
+      <c r="I33" s="53">
+        <f t="shared" si="4"/>
+        <v>1.3134180637906882E-2</v>
+      </c>
+      <c r="J33" s="25">
+        <f>IF(I33&gt;0, ('BPV Calcs'!$B$8/12)+(I33/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.32206417968622314</v>
+      </c>
+      <c r="K33" s="17"/>
+      <c r="L33" s="41">
         <f t="shared" si="0"/>
         <v>0.10253210256655709</v>
       </c>
-      <c r="G33" s="69">
-        <f>$M$7/((C33*(1-F33))+(D33*F33))</f>
+      <c r="M33" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H33" s="53">
-        <f t="shared" si="1"/>
+      <c r="N33" s="53">
+        <f t="shared" si="5"/>
         <v>7.7024675770458517E-2</v>
       </c>
-      <c r="I33" s="25">
-        <f>IF(H33&gt;$G$55, $G$58-(G33*(1-F33)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.70875065199591081</v>
-      </c>
-      <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O33" s="53">
+        <f t="shared" si="6"/>
+        <v>4.0036327297135764E-2</v>
+      </c>
+      <c r="P33" s="25">
+        <f>IF(I33&gt;0, ('BPV Calcs'!$B$8/12)+(O33/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.44833398532924401</v>
+      </c>
+      <c r="Q33" s="17"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
         <v>59</v>
       </c>
@@ -9600,26 +10580,51 @@
       <c r="D34" s="25">
         <v>0.26038490960479999</v>
       </c>
-      <c r="E34" s="17"/>
+      <c r="E34" s="53"/>
       <c r="F34" s="41">
+        <f t="shared" si="2"/>
+        <v>6.4516045601971481E-2</v>
+      </c>
+      <c r="G34" s="69">
+        <f>$T$7/((C34*(1-F34))+(D34*F34))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H34" s="53">
+        <f t="shared" si="3"/>
+        <v>4.7008670807325716E-2</v>
+      </c>
+      <c r="I34" s="53">
+        <f t="shared" si="4"/>
+        <v>1.0020322334002962E-2</v>
+      </c>
+      <c r="J34" s="25">
+        <f>IF(I34&gt;0, ('BPV Calcs'!$B$8/12)+(I34/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.30744875557846069</v>
+      </c>
+      <c r="K34" s="17"/>
+      <c r="L34" s="41">
         <f t="shared" si="0"/>
         <v>9.8524459836365458E-2</v>
       </c>
-      <c r="G34" s="69">
-        <f>$M$7/((C34*(1-F34))+(D34*F34))</f>
+      <c r="M34" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492435</v>
       </c>
-      <c r="H34" s="53">
-        <f t="shared" si="1"/>
+      <c r="N34" s="53">
+        <f t="shared" si="5"/>
         <v>7.4014034476952761E-2</v>
       </c>
-      <c r="I34" s="25">
-        <f>IF(H34&gt;$G$55, $G$58-(G34*(1-F34)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.69461969449994321</v>
-      </c>
-      <c r="J34" s="17"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O34" s="53">
+        <f t="shared" si="6"/>
+        <v>3.7025686003630008E-2</v>
+      </c>
+      <c r="P34" s="25">
+        <f>IF(I34&gt;0, ('BPV Calcs'!$B$8/12)+(O34/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.43420302783327736</v>
+      </c>
+      <c r="Q34" s="17"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <v>59.9</v>
       </c>
@@ -9632,26 +10637,51 @@
       <c r="D35" s="25">
         <v>0.26455302741599995</v>
       </c>
-      <c r="E35" s="17"/>
+      <c r="E35" s="53"/>
       <c r="F35" s="41">
+        <f t="shared" si="2"/>
+        <v>6.0121926464803473E-2</v>
+      </c>
+      <c r="G35" s="69">
+        <f>$T$7/((C35*(1-F35))+(D35*F35))</f>
+        <v>0.7286353397625045</v>
+      </c>
+      <c r="H35" s="53">
+        <f t="shared" si="3"/>
+        <v>4.3806960316858386E-2</v>
+      </c>
+      <c r="I35" s="53">
+        <f t="shared" si="4"/>
+        <v>6.8186118435356324E-3</v>
+      </c>
+      <c r="J35" s="25">
+        <f>IF(I35&gt;0, ('BPV Calcs'!$B$8/12)+(I35/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.29242098227555063</v>
+      </c>
+      <c r="K35" s="17"/>
+      <c r="L35" s="41">
         <f t="shared" si="0"/>
         <v>9.4404755900095283E-2</v>
       </c>
-      <c r="G35" s="69">
-        <f>$M$7/((C35*(1-F35))+(D35*F35))</f>
+      <c r="M35" s="69">
+        <f t="shared" si="1"/>
         <v>0.75122497093492435</v>
       </c>
-      <c r="H35" s="53">
-        <f t="shared" si="1"/>
+      <c r="N35" s="53">
+        <f t="shared" si="5"/>
         <v>7.0919210007167707E-2</v>
       </c>
-      <c r="I35" s="25">
-        <f>IF(H35&gt;$G$55, $G$58-(G35*(1-F35)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.68009360893327475</v>
-      </c>
-      <c r="J35" s="17"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O35" s="53">
+        <f t="shared" si="6"/>
+        <v>3.3930861533844954E-2</v>
+      </c>
+      <c r="P35" s="25">
+        <f>IF(I35&gt;0, ('BPV Calcs'!$B$8/12)+(O35/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.41967694226660884</v>
+      </c>
+      <c r="Q35" s="17"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
         <v>60.8</v>
       </c>
@@ -9664,26 +10694,51 @@
       <c r="D36" s="25">
         <v>0.2688100700928</v>
       </c>
-      <c r="E36" s="17"/>
+      <c r="E36" s="53"/>
       <c r="F36" s="41">
-        <f t="shared" ref="F36:F53" si="2">($C$53-C36)/(D36-C36)</f>
+        <f t="shared" si="2"/>
+        <v>5.5601372945089003E-2</v>
+      </c>
+      <c r="G36" s="69">
+        <f>$T$7/((C36*(1-F36))+(D36*F36))</f>
+        <v>0.7286353397625045</v>
+      </c>
+      <c r="H36" s="53">
+        <f t="shared" si="3"/>
+        <v>4.0513125267106653E-2</v>
+      </c>
+      <c r="I36" s="53">
+        <f t="shared" si="4"/>
+        <v>3.5247767937839E-3</v>
+      </c>
+      <c r="J36" s="25">
+        <f>IF(I36&gt;0, ('BPV Calcs'!$B$8/12)+(I36/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.27696080666872258</v>
+      </c>
+      <c r="K36" s="17"/>
+      <c r="L36" s="41">
+        <f t="shared" ref="L36:L53" si="7">($C$53-C36)/(D36-C36)</f>
         <v>9.0167576361954008E-2</v>
       </c>
-      <c r="G36" s="69">
-        <f>$M$7/((C36*(1-F36))+(D36*F36))</f>
+      <c r="M36" s="69">
+        <f t="shared" ref="M36:M67" si="8">$T$7/((C36*(1-L36))+(D36*L36))</f>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H36" s="53">
-        <f t="shared" si="1"/>
+      <c r="N36" s="53">
+        <f t="shared" si="5"/>
         <v>6.7736134931781461E-2</v>
       </c>
-      <c r="I36" s="25">
-        <f>IF(H36&gt;$G$55, $G$58-(G36*(1-F36)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.66515330412387197</v>
-      </c>
-      <c r="J36" s="17"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O36" s="53">
+        <f t="shared" si="6"/>
+        <v>3.0747786458458708E-2</v>
+      </c>
+      <c r="P36" s="25">
+        <f>IF(I36&gt;0, ('BPV Calcs'!$B$8/12)+(O36/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.40473663745720501</v>
+      </c>
+      <c r="Q36" s="17"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
         <v>61.7</v>
       </c>
@@ -9696,26 +10751,51 @@
       <c r="D37" s="25">
         <v>0.27315953021120004</v>
       </c>
-      <c r="E37" s="17"/>
+      <c r="E37" s="53"/>
       <c r="F37" s="41">
         <f t="shared" si="2"/>
+        <v>5.0946747774153422E-2</v>
+      </c>
+      <c r="G37" s="69">
+        <f>$T$7/((C37*(1-F37))+(D37*F37))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H37" s="53">
+        <f t="shared" si="3"/>
+        <v>3.7121600874214893E-2</v>
+      </c>
+      <c r="I37" s="53">
+        <f t="shared" si="4"/>
+        <v>1.332524008921393E-4</v>
+      </c>
+      <c r="J37" s="25">
+        <f>IF(I37&gt;0, ('BPV Calcs'!$B$8/12)+(I37/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.26104210949750278</v>
+      </c>
+      <c r="K37" s="17"/>
+      <c r="L37" s="41">
+        <f t="shared" si="7"/>
         <v>8.5805817247007074E-2</v>
       </c>
-      <c r="G37" s="69">
-        <f>$M$7/((C37*(1-F37))+(D37*F37))</f>
+      <c r="M37" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H37" s="53">
-        <f t="shared" si="1"/>
+      <c r="N37" s="53">
+        <f t="shared" si="5"/>
         <v>6.4459472567430315E-2</v>
       </c>
-      <c r="I37" s="25">
-        <f>IF(H37&gt;$G$55, $G$58-(G37*(1-F37)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.64977373143975337</v>
-      </c>
-      <c r="J37" s="17"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O37" s="53">
+        <f t="shared" si="6"/>
+        <v>2.7471124094107562E-2</v>
+      </c>
+      <c r="P37" s="25">
+        <f>IF(I37&gt;0, ('BPV Calcs'!$B$8/12)+(O37/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>0.38935706477308674</v>
+      </c>
+      <c r="Q37" s="17"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <v>62.6</v>
       </c>
@@ -9728,26 +10808,51 @@
       <c r="D38" s="25">
         <v>0.27760515258880003</v>
       </c>
-      <c r="E38" s="17"/>
+      <c r="E38" s="53"/>
       <c r="F38" s="41">
         <f t="shared" si="2"/>
+        <v>4.6149947630415508E-2</v>
+      </c>
+      <c r="G38" s="69">
+        <f>$T$7/((C38*(1-F38))+(D38*F38))</f>
+        <v>0.72863533976250427</v>
+      </c>
+      <c r="H38" s="53">
+        <f t="shared" si="3"/>
+        <v>3.3626482771709584E-2</v>
+      </c>
+      <c r="I38" s="53">
+        <f t="shared" si="4"/>
+        <v>-3.3618657016131689E-3</v>
+      </c>
+      <c r="J38" s="25" t="str">
+        <f>IF(I38&gt;0, ('BPV Calcs'!$B$8/12)+(I38/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K38" s="17"/>
+      <c r="L38" s="41">
+        <f t="shared" si="7"/>
         <v>8.1311947956176495E-2</v>
       </c>
-      <c r="G38" s="69">
-        <f>$M$7/((C38*(1-F38))+(D38*F38))</f>
+      <c r="M38" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H38" s="53">
-        <f t="shared" si="1"/>
+      <c r="N38" s="53">
+        <f t="shared" si="5"/>
         <v>6.1083565740040757E-2</v>
       </c>
-      <c r="I38" s="25">
-        <f>IF(H38&gt;$G$55, $G$58-(G38*(1-F38)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.63392833797122883</v>
-      </c>
-      <c r="J38" s="17"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O38" s="53">
+        <f t="shared" si="6"/>
+        <v>2.4095217266718004E-2</v>
+      </c>
+      <c r="P38" s="25" t="str">
+        <f>IF(I38&gt;0, ('BPV Calcs'!$B$8/12)+(O38/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="Q38" s="17"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
         <v>63.5</v>
       </c>
@@ -9760,26 +10865,51 @@
       <c r="D39" s="25">
         <v>0.28215091488159999</v>
       </c>
-      <c r="E39" s="17"/>
+      <c r="E39" s="53"/>
       <c r="F39" s="41">
         <f t="shared" si="2"/>
+        <v>4.1202358029293618E-2</v>
+      </c>
+      <c r="G39" s="69">
+        <f>$T$7/((C39*(1-F39))+(D39*F39))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H39" s="53">
+        <f t="shared" si="3"/>
+        <v>3.0021494141690707E-2</v>
+      </c>
+      <c r="I39" s="53">
+        <f t="shared" si="4"/>
+        <v>-6.9668543316320462E-3</v>
+      </c>
+      <c r="J39" s="25" t="str">
+        <f>IF(I39&gt;0, ('BPV Calcs'!$B$8/12)+(I39/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K39" s="17"/>
+      <c r="L39" s="41">
+        <f t="shared" si="7"/>
         <v>7.6677969006389013E-2</v>
       </c>
-      <c r="G39" s="69">
-        <f>$M$7/((C39*(1-F39))+(D39*F39))</f>
+      <c r="M39" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H39" s="53">
-        <f t="shared" si="1"/>
+      <c r="N39" s="53">
+        <f t="shared" si="5"/>
         <v>5.7602405038173606E-2</v>
       </c>
-      <c r="I39" s="25">
-        <f>IF(H39&gt;$G$55, $G$58-(G39*(1-F39)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.61758891752256018</v>
-      </c>
-      <c r="J39" s="17"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O39" s="53">
+        <f t="shared" si="6"/>
+        <v>2.0614056564850852E-2</v>
+      </c>
+      <c r="P39" s="25" t="str">
+        <f>IF(I39&gt;0, ('BPV Calcs'!$B$8/12)+(O39/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="Q39" s="17"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
         <v>64.400000000000006</v>
       </c>
@@ -9792,26 +10922,51 @@
       <c r="D40" s="25">
         <v>0.28680106639039998</v>
       </c>
-      <c r="E40" s="17"/>
+      <c r="E40" s="53"/>
       <c r="F40" s="41">
         <f t="shared" si="2"/>
+        <v>3.6096283439178707E-2</v>
+      </c>
+      <c r="G40" s="69">
+        <f>$T$7/((C40*(1-F40))+(D40*F40))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H40" s="53">
+        <f t="shared" si="3"/>
+        <v>2.6301027747869639E-2</v>
+      </c>
+      <c r="I40" s="53">
+        <f t="shared" si="4"/>
+        <v>-1.0687320725453114E-2</v>
+      </c>
+      <c r="J40" s="25" t="str">
+        <f>IF(I40&gt;0, ('BPV Calcs'!$B$8/12)+(I40/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K40" s="17"/>
+      <c r="L40" s="41">
+        <f t="shared" si="7"/>
         <v>7.1896792063500151E-2</v>
       </c>
-      <c r="G40" s="69">
-        <f>$M$7/((C40*(1-F40))+(D40*F40))</f>
+      <c r="M40" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H40" s="53">
-        <f t="shared" si="1"/>
+      <c r="N40" s="53">
+        <f t="shared" si="5"/>
         <v>5.4010665528217192E-2</v>
       </c>
-      <c r="I40" s="25">
-        <f>IF(H40&gt;$G$55, $G$58-(G40*(1-F40)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.60073047661123002</v>
-      </c>
-      <c r="J40" s="17"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O40" s="53">
+        <f t="shared" si="6"/>
+        <v>1.7022317054894438E-2</v>
+      </c>
+      <c r="P40" s="25" t="str">
+        <f>IF(I40&gt;0, ('BPV Calcs'!$B$8/12)+(O40/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="Q40" s="17"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
         <v>65.3</v>
       </c>
@@ -9824,26 +10979,51 @@
       <c r="D41" s="25">
         <v>0.29156020567359997</v>
       </c>
-      <c r="E41" s="17"/>
+      <c r="E41" s="53"/>
       <c r="F41" s="41">
         <f t="shared" si="2"/>
+        <v>3.0819003777835637E-2</v>
+      </c>
+      <c r="G41" s="69">
+        <f>$T$7/((C41*(1-F41))+(D41*F41))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H41" s="53">
+        <f t="shared" si="3"/>
+        <v>2.2455815288805175E-2</v>
+      </c>
+      <c r="I41" s="53">
+        <f t="shared" si="4"/>
+        <v>-1.4532533184517579E-2</v>
+      </c>
+      <c r="J41" s="25" t="str">
+        <f>IF(I41&gt;0, ('BPV Calcs'!$B$8/12)+(I41/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K41" s="17"/>
+      <c r="L41" s="41">
+        <f t="shared" si="7"/>
         <v>6.6956521460969767E-2</v>
       </c>
-      <c r="G41" s="69">
-        <f>$M$7/((C41*(1-F41))+(D41*F41))</f>
+      <c r="M41" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H41" s="53">
-        <f t="shared" si="1"/>
+      <c r="N41" s="53">
+        <f t="shared" si="5"/>
         <v>5.0299410888420645E-2</v>
       </c>
-      <c r="I41" s="25">
-        <f>IF(H41&gt;$G$55, $G$58-(G41*(1-F41)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.58331107108962232</v>
-      </c>
-      <c r="J41" s="17"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O41" s="53">
+        <f t="shared" si="6"/>
+        <v>1.3311062415097892E-2</v>
+      </c>
+      <c r="P41" s="25" t="str">
+        <f>IF(I41&gt;0, ('BPV Calcs'!$B$8/12)+(O41/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="Q41" s="17"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
         <v>66.2</v>
       </c>
@@ -9856,26 +11036,51 @@
       <c r="D42" s="25">
         <v>0.29643326114399998</v>
       </c>
-      <c r="E42" s="17"/>
+      <c r="E42" s="53"/>
       <c r="F42" s="41">
         <f t="shared" si="2"/>
+        <v>2.5359990565452944E-2</v>
+      </c>
+      <c r="G42" s="69">
+        <f>$T$7/((C42*(1-F42))+(D42*F42))</f>
+        <v>0.72863533976250427</v>
+      </c>
+      <c r="H42" s="53">
+        <f t="shared" si="3"/>
+        <v>1.8478185342032709E-2</v>
+      </c>
+      <c r="I42" s="53">
+        <f t="shared" si="4"/>
+        <v>-1.8510163131290044E-2</v>
+      </c>
+      <c r="J42" s="25" t="str">
+        <f>IF(I42&gt;0, ('BPV Calcs'!$B$8/12)+(I42/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K42" s="17"/>
+      <c r="L42" s="41">
+        <f t="shared" si="7"/>
         <v>6.1847405437448669E-2</v>
       </c>
-      <c r="G42" s="69">
-        <f>$M$7/((C42*(1-F42))+(D42*F42))</f>
+      <c r="M42" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H42" s="53">
-        <f t="shared" si="1"/>
+      <c r="N42" s="53">
+        <f t="shared" si="5"/>
         <v>4.6461315352147849E-2</v>
       </c>
-      <c r="I42" s="25">
-        <f>IF(H42&gt;$G$55, $G$58-(G42*(1-F42)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.56529631622476284</v>
-      </c>
-      <c r="J42" s="17"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O42" s="53">
+        <f t="shared" si="6"/>
+        <v>9.4729668788250954E-3</v>
+      </c>
+      <c r="P42" s="25" t="str">
+        <f>IF(I42&gt;0, ('BPV Calcs'!$B$8/12)+(O42/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="Q42" s="17"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
         <v>67.099999999999994</v>
       </c>
@@ -9888,26 +11093,51 @@
       <c r="D43" s="25">
         <v>0.301425510472</v>
       </c>
-      <c r="E43" s="17"/>
+      <c r="E43" s="53"/>
       <c r="F43" s="41">
         <f t="shared" si="2"/>
+        <v>1.9707963149169245E-2</v>
+      </c>
+      <c r="G43" s="69">
+        <f>$T$7/((C43*(1-F43))+(D43*F43))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H43" s="53">
+        <f t="shared" si="3"/>
+        <v>1.4359918425221848E-2</v>
+      </c>
+      <c r="I43" s="53">
+        <f t="shared" si="4"/>
+        <v>-2.2628430048100903E-2</v>
+      </c>
+      <c r="J43" s="25" t="str">
+        <f>IF(I43&gt;0, ('BPV Calcs'!$B$8/12)+(I43/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K43" s="17"/>
+      <c r="L43" s="41">
+        <f t="shared" si="7"/>
         <v>5.6559004365802502E-2</v>
       </c>
-      <c r="G43" s="69">
-        <f>$M$7/((C43*(1-F43))+(D43*F43))</f>
+      <c r="M43" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H43" s="53">
-        <f t="shared" si="1"/>
+      <c r="N43" s="53">
+        <f t="shared" si="5"/>
         <v>4.2488536410808235E-2</v>
       </c>
-      <c r="I43" s="25">
-        <f>IF(H43&gt;$G$55, $G$58-(G43*(1-F43)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.54664940186733357</v>
-      </c>
-      <c r="J43" s="17"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O43" s="53">
+        <f t="shared" si="6"/>
+        <v>5.5001879374854817E-3</v>
+      </c>
+      <c r="P43" s="25" t="str">
+        <f>IF(I43&gt;0, ('BPV Calcs'!$B$8/12)+(O43/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="Q43" s="17"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
         <v>68</v>
       </c>
@@ -9920,26 +11150,51 @@
       <c r="D44" s="25">
         <v>0.30654265819839999</v>
       </c>
-      <c r="E44" s="17"/>
+      <c r="E44" s="53"/>
       <c r="F44" s="41">
         <f t="shared" si="2"/>
+        <v>1.3849237062883164E-2</v>
+      </c>
+      <c r="G44" s="69">
+        <f>$T$7/((C44*(1-F44))+(D44*F44))</f>
+        <v>0.7286353397625045</v>
+      </c>
+      <c r="H44" s="53">
+        <f t="shared" si="3"/>
+        <v>1.0091043552765345E-2</v>
+      </c>
+      <c r="I44" s="53">
+        <f t="shared" si="4"/>
+        <v>-2.6897304920557408E-2</v>
+      </c>
+      <c r="J44" s="25" t="str">
+        <f>IF(I44&gt;0, ('BPV Calcs'!$B$8/12)+(I44/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K44" s="17"/>
+      <c r="L44" s="41">
+        <f t="shared" si="7"/>
         <v>5.1078607093820678E-2</v>
       </c>
-      <c r="G44" s="69">
-        <f>$M$7/((C44*(1-F44))+(D44*F44))</f>
+      <c r="M44" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H44" s="53">
-        <f t="shared" si="1"/>
+      <c r="N44" s="53">
+        <f t="shared" si="5"/>
         <v>3.8371525129451856E-2</v>
       </c>
-      <c r="I44" s="25">
-        <f>IF(H44&gt;$G$55, $G$58-(G44*(1-F44)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
-        <v>0.52732550846536741</v>
-      </c>
-      <c r="J44" s="17"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O44" s="53">
+        <f t="shared" si="6"/>
+        <v>1.3831766561291023E-3</v>
+      </c>
+      <c r="P44" s="25" t="str">
+        <f>IF(I44&gt;0, ('BPV Calcs'!$B$8/12)+(O44/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="Q44" s="17"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
         <v>68.900000000000006</v>
       </c>
@@ -9952,26 +11207,51 @@
       <c r="D45" s="25">
         <v>0.31179093275039999</v>
       </c>
-      <c r="E45" s="17"/>
+      <c r="E45" s="53"/>
       <c r="F45" s="41">
         <f t="shared" si="2"/>
+        <v>7.7675006515787424E-3</v>
+      </c>
+      <c r="G45" s="69">
+        <f>$T$7/((C45*(1-F45))+(D45*F45))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H45" s="53">
+        <f t="shared" si="3"/>
+        <v>5.6596754763685508E-3</v>
+      </c>
+      <c r="I45" s="53">
+        <f t="shared" si="4"/>
+        <v>-3.1328672996954202E-2</v>
+      </c>
+      <c r="J45" s="25" t="str">
+        <f>IF(I45&gt;0, ('BPV Calcs'!$B$8/12)+(I45/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K45" s="17"/>
+      <c r="L45" s="41">
+        <f t="shared" si="7"/>
         <v>4.5391024185220959E-2</v>
       </c>
-      <c r="G45" s="69">
-        <f>$M$7/((C45*(1-F45))+(D45*F45))</f>
+      <c r="M45" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492435</v>
       </c>
-      <c r="H45" s="53">
-        <f t="shared" si="1"/>
+      <c r="N45" s="53">
+        <f t="shared" si="5"/>
         <v>3.4098870824249061E-2</v>
       </c>
-      <c r="I45" s="25" t="str">
-        <f>IF(H45&gt;$G$55, $G$58-(G45*(1-F45)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
+      <c r="O45" s="53">
+        <f t="shared" si="6"/>
+        <v>-2.889477649073692E-3</v>
+      </c>
+      <c r="P45" s="25" t="str">
+        <f>IF(I45&gt;0, ('BPV Calcs'!$B$8/12)+(O45/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
         <v>SEE EQN in Notes</v>
       </c>
-      <c r="J45" s="17"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q45" s="17"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
         <v>69.8</v>
       </c>
@@ -9984,26 +11264,51 @@
       <c r="D46" s="25">
         <v>0.31717698942559996</v>
       </c>
-      <c r="E46" s="17"/>
+      <c r="E46" s="53"/>
       <c r="F46" s="41">
         <f t="shared" si="2"/>
+        <v>1.4484372022368131E-3</v>
+      </c>
+      <c r="G46" s="69">
+        <f>$T$7/((C46*(1-F46))+(D46*F46))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H46" s="53">
+        <f>G46*F46</f>
+        <v>1.0553825329764717E-3</v>
+      </c>
+      <c r="I46" s="53">
+        <f t="shared" si="4"/>
+        <v>-3.5932965940346284E-2</v>
+      </c>
+      <c r="J46" s="25" t="str">
+        <f>IF(I46&gt;0, ('BPV Calcs'!$B$8/12)+(I46/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K46" s="17"/>
+      <c r="L46" s="41">
+        <f t="shared" si="7"/>
         <v>3.9483036942300216E-2</v>
       </c>
-      <c r="G46" s="69">
-        <f>$M$7/((C46*(1-F46))+(D46*F46))</f>
+      <c r="M46" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492435</v>
       </c>
-      <c r="H46" s="53">
-        <f t="shared" si="1"/>
+      <c r="N46" s="53">
+        <f t="shared" si="5"/>
         <v>2.9660643279402023E-2</v>
       </c>
-      <c r="I46" s="25" t="str">
-        <f>IF(H46&gt;$G$55, $G$58-(G46*(1-F46)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
+      <c r="O46" s="53">
+        <f t="shared" si="6"/>
+        <v>-7.3277051939207305E-3</v>
+      </c>
+      <c r="P46" s="25" t="str">
+        <f>IF(I46&gt;0, ('BPV Calcs'!$B$8/12)+(O46/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
         <v>SEE EQN in Notes</v>
       </c>
-      <c r="J46" s="17"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q46" s="17"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="70">
         <v>70</v>
       </c>
@@ -10019,28 +11324,53 @@
         <f>D46+(((D48-D46)/($A$48-$A$46))*($A$47-$A$46))</f>
         <v>0.31840613902737774</v>
       </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="72">
-        <f t="shared" si="2"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="41">
+        <f>($C$47-C47)/(D47-C47)</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="69">
+        <f>$T$7/((C47*(1-F47))+(D47*F47))</f>
+        <v>0.72863533976250439</v>
+      </c>
+      <c r="H47" s="53">
+        <f>G47*F47</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="53">
+        <f t="shared" si="4"/>
+        <v>-3.6988348473322753E-2</v>
+      </c>
+      <c r="J47" s="25" t="str">
+        <f>IF(I47&gt;0, ('BPV Calcs'!$B$8/12)+(I47/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
+        <v>SEE EQN in Notes</v>
+      </c>
+      <c r="K47" s="17"/>
+      <c r="L47" s="72">
+        <f t="shared" si="7"/>
         <v>3.8129176343576189E-2</v>
       </c>
-      <c r="G47" s="73">
-        <f>$M$7/((C47*(1-F47))+(D47*F47))</f>
+      <c r="M47" s="73">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H47" s="50">
-        <f t="shared" si="1"/>
+      <c r="N47" s="50">
+        <f t="shared" si="5"/>
         <v>2.8643589390475625E-2</v>
       </c>
-      <c r="I47" s="45" t="str">
-        <f>IF(H47&gt;$G$55, $G$58-(G47*(1-F47)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
+      <c r="O47" s="53">
+        <f t="shared" si="6"/>
+        <v>-8.3447590828471287E-3</v>
+      </c>
+      <c r="P47" s="25" t="str">
+        <f>IF(I47&gt;0, ('BPV Calcs'!$B$8/12)+(O47/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
         <v>SEE EQN in Notes</v>
       </c>
-      <c r="J47" s="17"/>
-      <c r="K47" s="42"/>
-      <c r="L47" s="52"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q47" s="17"/>
+      <c r="R47" s="52"/>
+      <c r="S47" s="52"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
         <v>70.7</v>
       </c>
@@ -10053,26 +11383,36 @@
       <c r="D48" s="25">
         <v>0.32270816263359997</v>
       </c>
-      <c r="E48" s="17"/>
-      <c r="F48" s="41">
-        <f t="shared" si="2"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="41">
+        <f t="shared" si="7"/>
         <v>3.3337176339955747E-2</v>
       </c>
-      <c r="G48" s="69">
-        <f>$M$7/((C48*(1-F48))+(D48*F48))</f>
+      <c r="M48" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H48" s="53">
-        <f t="shared" si="1"/>
+      <c r="N48" s="53">
+        <f t="shared" si="5"/>
         <v>2.50437193270357E-2</v>
       </c>
-      <c r="I48" s="25" t="str">
-        <f>IF(H48&gt;$G$55, $G$58-(G48*(1-F48)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
+      <c r="O48" s="53">
+        <f t="shared" si="6"/>
+        <v>-1.1944629146287054E-2</v>
+      </c>
+      <c r="P48" s="25" t="str">
+        <f>IF(I48&gt;0, ('BPV Calcs'!$B$8/12)+(O48/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
         <v>SEE EQN in Notes</v>
       </c>
-      <c r="J48" s="17"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q48" s="17"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
         <v>71.599999999999994</v>
       </c>
@@ -10085,26 +11425,36 @@
       <c r="D49" s="25">
         <v>0.32839236888000001</v>
       </c>
-      <c r="E49" s="17"/>
-      <c r="F49" s="41">
-        <f t="shared" si="2"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="41">
+        <f t="shared" si="7"/>
         <v>2.693291798927008E-2</v>
       </c>
-      <c r="G49" s="69">
-        <f>$M$7/((C49*(1-F49))+(D49*F49))</f>
+      <c r="M49" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H49" s="53">
-        <f t="shared" si="1"/>
+      <c r="N49" s="53">
+        <f t="shared" si="5"/>
         <v>2.0232680533682115E-2</v>
       </c>
-      <c r="I49" s="25" t="str">
-        <f>IF(H49&gt;$G$55, $G$58-(G49*(1-F49)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
+      <c r="O49" s="53">
+        <f t="shared" si="6"/>
+        <v>-1.6755667939640638E-2</v>
+      </c>
+      <c r="P49" s="25" t="str">
+        <f>IF(I49&gt;0, ('BPV Calcs'!$B$8/12)+(O49/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
         <v>SEE EQN in Notes</v>
       </c>
-      <c r="J49" s="17"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q49" s="17"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
         <v>72.5</v>
       </c>
@@ -10117,26 +11467,36 @@
       <c r="D50" s="25">
         <v>0.33423830079839995</v>
       </c>
-      <c r="E50" s="17"/>
-      <c r="F50" s="41">
-        <f t="shared" si="2"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="41">
+        <f t="shared" si="7"/>
         <v>2.0249656851450533E-2</v>
       </c>
-      <c r="G50" s="69">
-        <f>$M$7/((C50*(1-F50))+(D50*F50))</f>
+      <c r="M50" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H50" s="53">
-        <f t="shared" si="1"/>
+      <c r="N50" s="53">
+        <f t="shared" si="5"/>
         <v>1.5212047879673117E-2</v>
       </c>
-      <c r="I50" s="25" t="str">
-        <f>IF(H50&gt;$G$55, $G$58-(G50*(1-F50)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
+      <c r="O50" s="53">
+        <f t="shared" si="6"/>
+        <v>-2.1776300593649635E-2</v>
+      </c>
+      <c r="P50" s="25" t="str">
+        <f>IF(I50&gt;0, ('BPV Calcs'!$B$8/12)+(O50/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
         <v>SEE EQN in Notes</v>
       </c>
-      <c r="J50" s="17"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q50" s="17"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
         <v>73.400000000000006</v>
       </c>
@@ -10149,26 +11509,36 @@
       <c r="D51" s="25">
         <v>0.34025552416639998</v>
       </c>
-      <c r="E51" s="17"/>
-      <c r="F51" s="41">
-        <f t="shared" si="2"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="53"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="41">
+        <f t="shared" si="7"/>
         <v>1.3264956550221583E-2</v>
       </c>
-      <c r="G51" s="69">
-        <f>$M$7/((C51*(1-F51))+(D51*F51))</f>
+      <c r="M51" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H51" s="53">
-        <f t="shared" si="1"/>
+      <c r="N51" s="53">
+        <f t="shared" si="5"/>
         <v>9.964966598893241E-3</v>
       </c>
-      <c r="I51" s="25" t="str">
-        <f>IF(H51&gt;$G$55, $G$58-(G51*(1-F51)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
+      <c r="O51" s="53">
+        <f t="shared" si="6"/>
+        <v>-2.7023381874429514E-2</v>
+      </c>
+      <c r="P51" s="25" t="str">
+        <f>IF(I51&gt;0, ('BPV Calcs'!$B$8/12)+(O51/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
         <v>SEE EQN in Notes</v>
       </c>
-      <c r="J51" s="17"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q51" s="17"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="27">
         <v>74.3</v>
       </c>
@@ -10181,26 +11551,36 @@
       <c r="D52" s="25">
         <v>0.34645449730880001</v>
       </c>
-      <c r="E52" s="17"/>
-      <c r="F52" s="41">
-        <f t="shared" si="2"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="69"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="41">
+        <f t="shared" si="7"/>
         <v>5.9508601980526824E-3</v>
       </c>
-      <c r="G52" s="69">
-        <f>$M$7/((C52*(1-F52))+(D52*F52))</f>
+      <c r="M52" s="69">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H52" s="53">
-        <f t="shared" si="1"/>
+      <c r="N52" s="53">
+        <f t="shared" si="5"/>
         <v>4.4704347793199243E-3</v>
       </c>
-      <c r="I52" s="25" t="str">
-        <f>IF(H52&gt;$G$55, $G$58-(G52*(1-F52)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
+      <c r="O52" s="53">
+        <f t="shared" si="6"/>
+        <v>-3.251791369400283E-2</v>
+      </c>
+      <c r="P52" s="25" t="str">
+        <f>IF(I52&gt;0, ('BPV Calcs'!$B$8/12)+(O52/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
         <v>SEE EQN in Notes</v>
       </c>
-      <c r="J52" s="17"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q52" s="17"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="70">
         <v>75</v>
       </c>
@@ -10209,35 +11589,45 @@
         <v>799.74517236666668</v>
       </c>
       <c r="C53" s="44">
-        <f t="shared" ref="C53:D53" si="3">C52+(((C54-C52)/($A$54-$A$52))*($A$53-$A$52))</f>
+        <f t="shared" ref="C53:D53" si="9">C52+(((C54-C52)/($A$54-$A$52))*($A$53-$A$52))</f>
         <v>1.4612000162666667</v>
       </c>
       <c r="D53" s="45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.35142632153493331</v>
       </c>
-      <c r="E53" s="53"/>
-      <c r="F53" s="74">
-        <f t="shared" si="2"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="50"/>
+      <c r="J53" s="50"/>
+      <c r="K53" s="53"/>
+      <c r="L53" s="74">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G53" s="75">
-        <f>$M$7/((C53*(1-F53))+(D53*F53))</f>
+      <c r="M53" s="75">
+        <f t="shared" si="8"/>
         <v>0.75122497093492424</v>
       </c>
-      <c r="H53" s="76">
-        <f t="shared" si="1"/>
+      <c r="N53" s="76">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I53" s="45" t="str">
-        <f>IF(H53&gt;$G$55, $G$58-(G53*(1-F53)-$G$55)/(PI()*('BPV Calcs'!$B$8/12)^2), "SEE EQN in Notes")</f>
+      <c r="O53" s="53">
+        <f t="shared" si="6"/>
+        <v>-3.6988348473322753E-2</v>
+      </c>
+      <c r="P53" s="25" t="str">
+        <f>IF(I53&gt;0, ('BPV Calcs'!$B$8/12)+(O53/(PI()*(('BPV Calcs'!$B$8/12)^2))), "SEE EQN in Notes")</f>
         <v>SEE EQN in Notes</v>
       </c>
-      <c r="J53" s="53"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="43"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q53" s="53"/>
+      <c r="R53" s="43"/>
+      <c r="S53" s="43"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
         <v>75.2</v>
       </c>
@@ -10250,14 +11640,21 @@
       <c r="D54" s="25">
         <v>0.35284684274239997</v>
       </c>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
-      <c r="J54" s="17"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="17"/>
+      <c r="Q54" s="17"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
         <v>76.099999999999994</v>
       </c>
@@ -10270,19 +11667,26 @@
       <c r="D55" s="25">
         <v>0.35944542478879998</v>
       </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G55" s="17">
-        <f>(2/3)*PI()*(('BPV Calcs'!B8/12)^3)</f>
-        <v>3.6988348473322753E-2</v>
-      </c>
+      <c r="E55" s="53"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
       <c r="H55" s="17"/>
       <c r="I55" s="17"/>
       <c r="J55" s="17"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K55" s="17"/>
+      <c r="L55" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M55" s="17">
+        <f>(2/3)*PI()*(('BPV Calcs'!B8/12)^3)</f>
+        <v>3.6988348473322753E-2</v>
+      </c>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
         <v>77</v>
       </c>
@@ -10295,19 +11699,26 @@
       <c r="D56" s="25">
         <v>0.36626458241279997</v>
       </c>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G56" s="17">
-        <f>G4-(2*G55)</f>
-        <v>0.67724827398827869</v>
-      </c>
+      <c r="E56" s="53"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
       <c r="H56" s="17"/>
       <c r="I56" s="17"/>
       <c r="J56" s="17"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K56" s="17"/>
+      <c r="L56" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="M56" s="17">
+        <f>M4-(2*M55)</f>
+        <v>0.67724827398827869</v>
+      </c>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
         <v>77.900000000000006</v>
       </c>
@@ -10320,19 +11731,26 @@
       <c r="D57" s="25">
         <v>0.37332036206079999</v>
       </c>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G57" s="17">
-        <f>G56/(PI()*(('BPV Calcs'!B8/12)^2))</f>
-        <v>3.1787800807053701</v>
-      </c>
+      <c r="E57" s="53"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
       <c r="H57" s="17"/>
       <c r="I57" s="17"/>
       <c r="J57" s="17"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K57" s="17"/>
+      <c r="L57" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M57" s="17">
+        <f>M56/(PI()*(('BPV Calcs'!B8/12)^2))</f>
+        <v>3.1787800807053701</v>
+      </c>
+      <c r="N57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
         <v>78.8</v>
       </c>
@@ -10345,19 +11763,26 @@
       <c r="D58" s="25">
         <v>0.38063080870880001</v>
       </c>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G58" s="17">
-        <f>G57+(2*'BPV Calcs'!B8/12)</f>
-        <v>3.6996134140387036</v>
-      </c>
+      <c r="E58" s="53"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
       <c r="H58" s="17"/>
       <c r="I58" s="17"/>
       <c r="J58" s="17"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K58" s="17"/>
+      <c r="L58" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="M58" s="17">
+        <f>M57+(2*'BPV Calcs'!B8/12)</f>
+        <v>3.6996134140387036</v>
+      </c>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
         <v>79.7</v>
       </c>
@@ -10370,14 +11795,21 @@
       <c r="D59" s="25">
         <v>0.38821637332959996</v>
       </c>
-      <c r="E59" s="17"/>
+      <c r="E59" s="53"/>
       <c r="F59" s="17"/>
       <c r="G59" s="17"/>
       <c r="H59" s="17"/>
       <c r="I59" s="17"/>
       <c r="J59" s="17"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
         <v>80.599999999999994</v>
       </c>
@@ -10390,14 +11822,21 @@
       <c r="D60" s="25">
         <v>0.3961002815536</v>
       </c>
-      <c r="E60" s="17"/>
-      <c r="F60" s="81"/>
-      <c r="G60" s="81"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="94"/>
+      <c r="G60" s="94"/>
       <c r="H60" s="17"/>
       <c r="I60" s="17"/>
       <c r="J60" s="17"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K60" s="17"/>
+      <c r="L60" s="94"/>
+      <c r="M60" s="94"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="17"/>
+      <c r="P60" s="17"/>
+      <c r="Q60" s="17"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
         <v>81.5</v>
       </c>
@@ -10410,14 +11849,21 @@
       <c r="D61" s="25">
         <v>0.40430919337760002</v>
       </c>
-      <c r="E61" s="17"/>
+      <c r="E61" s="53"/>
       <c r="F61" s="17"/>
       <c r="G61" s="17"/>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
       <c r="J61" s="17"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K61" s="17"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="17"/>
+      <c r="P61" s="17"/>
+      <c r="Q61" s="17"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
         <v>82.4</v>
       </c>
@@ -10430,14 +11876,21 @@
       <c r="D62" s="25">
         <v>0.41287390167999999</v>
       </c>
-      <c r="E62" s="17"/>
+      <c r="E62" s="53"/>
       <c r="F62" s="17"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
       <c r="J62" s="17"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="17"/>
+      <c r="O62" s="17"/>
+      <c r="P62" s="17"/>
+      <c r="Q62" s="17"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="27">
         <v>83.3</v>
       </c>
@@ -10450,14 +11903,21 @@
       <c r="D63" s="25">
         <v>0.42183024417120002</v>
       </c>
-      <c r="E63" s="17"/>
+      <c r="E63" s="53"/>
       <c r="F63" s="17"/>
       <c r="G63" s="17"/>
       <c r="H63" s="17"/>
       <c r="I63" s="17"/>
       <c r="J63" s="17"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="17"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
         <v>84.2</v>
       </c>
@@ -10470,14 +11930,21 @@
       <c r="D64" s="25">
         <v>0.43122034519840002</v>
       </c>
-      <c r="E64" s="17"/>
+      <c r="E64" s="53"/>
       <c r="F64" s="17"/>
       <c r="G64" s="17"/>
       <c r="H64" s="17"/>
       <c r="I64" s="17"/>
       <c r="J64" s="17"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="17"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
         <v>85.1</v>
       </c>
@@ -10490,14 +11957,21 @@
       <c r="D65" s="25">
         <v>0.44109424561439997</v>
       </c>
-      <c r="E65" s="17"/>
+      <c r="E65" s="53"/>
       <c r="F65" s="17"/>
       <c r="G65" s="17"/>
       <c r="H65" s="17"/>
       <c r="I65" s="17"/>
       <c r="J65" s="17"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="17"/>
+      <c r="O65" s="17"/>
+      <c r="P65" s="17"/>
+      <c r="Q65" s="17"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="27">
         <v>86</v>
       </c>
@@ -10510,14 +11984,21 @@
       <c r="D66" s="25">
         <v>0.45151211474239994</v>
       </c>
-      <c r="E66" s="17"/>
+      <c r="E66" s="53"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
       <c r="H66" s="17"/>
       <c r="I66" s="17"/>
       <c r="J66" s="17"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="17"/>
+      <c r="O66" s="17"/>
+      <c r="P66" s="17"/>
+      <c r="Q66" s="17"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
         <v>86.9</v>
       </c>
@@ -10530,14 +12011,21 @@
       <c r="D67" s="25">
         <v>0.4625472966784</v>
       </c>
-      <c r="E67" s="17"/>
+      <c r="E67" s="53"/>
       <c r="F67" s="17"/>
       <c r="G67" s="17"/>
       <c r="H67" s="17"/>
       <c r="I67" s="17"/>
       <c r="J67" s="17"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="17"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
         <v>87.8</v>
       </c>
@@ -10550,14 +12038,21 @@
       <c r="D68" s="25">
         <v>0.47429065660800002</v>
       </c>
-      <c r="E68" s="17"/>
+      <c r="E68" s="53"/>
       <c r="F68" s="17"/>
       <c r="G68" s="17"/>
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
       <c r="J68" s="17"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K68" s="17"/>
+      <c r="L68" s="17"/>
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
+      <c r="O68" s="17"/>
+      <c r="P68" s="17"/>
+      <c r="Q68" s="17"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
         <v>88.7</v>
       </c>
@@ -10570,14 +12065,21 @@
       <c r="D69" s="25">
         <v>0.48685690624959999</v>
       </c>
-      <c r="E69" s="17"/>
+      <c r="E69" s="53"/>
       <c r="F69" s="17"/>
       <c r="G69" s="17"/>
       <c r="H69" s="17"/>
       <c r="I69" s="17"/>
       <c r="J69" s="17"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K69" s="17"/>
+      <c r="L69" s="17"/>
+      <c r="M69" s="17"/>
+      <c r="N69" s="17"/>
+      <c r="O69" s="17"/>
+      <c r="P69" s="17"/>
+      <c r="Q69" s="17"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
         <v>89.6</v>
       </c>
@@ -10590,14 +12092,21 @@
       <c r="D70" s="25">
         <v>0.50039415022879996</v>
       </c>
-      <c r="E70" s="17"/>
+      <c r="E70" s="53"/>
       <c r="F70" s="17"/>
       <c r="G70" s="17"/>
       <c r="H70" s="17"/>
       <c r="I70" s="17"/>
       <c r="J70" s="17"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K70" s="17"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="17"/>
+      <c r="Q70" s="17"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
         <v>90.5</v>
       </c>
@@ -10610,14 +12119,21 @@
       <c r="D71" s="25">
         <v>0.51509886534880001</v>
       </c>
-      <c r="E71" s="17"/>
+      <c r="E71" s="53"/>
       <c r="F71" s="17"/>
       <c r="G71" s="17"/>
       <c r="H71" s="17"/>
       <c r="I71" s="17"/>
       <c r="J71" s="17"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K71" s="17"/>
+      <c r="L71" s="17"/>
+      <c r="M71" s="17"/>
+      <c r="N71" s="17"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
+      <c r="Q71" s="17"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="27">
         <v>91.4</v>
       </c>
@@ -10630,14 +12146,21 @@
       <c r="D72" s="25">
         <v>0.53124065907359996</v>
       </c>
-      <c r="E72" s="17"/>
+      <c r="E72" s="53"/>
       <c r="F72" s="17"/>
       <c r="G72" s="17"/>
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
       <c r="J72" s="17"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K72" s="17"/>
+      <c r="L72" s="17"/>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
+      <c r="Q72" s="17"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
         <v>92.3</v>
       </c>
@@ -10650,14 +12173,21 @@
       <c r="D73" s="25">
         <v>0.54920555806720006</v>
       </c>
-      <c r="E73" s="17"/>
+      <c r="E73" s="53"/>
       <c r="F73" s="17"/>
       <c r="G73" s="17"/>
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
       <c r="J73" s="17"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K73" s="17"/>
+      <c r="L73" s="17"/>
+      <c r="M73" s="17"/>
+      <c r="N73" s="17"/>
+      <c r="O73" s="17"/>
+      <c r="P73" s="17"/>
+      <c r="Q73" s="17"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
         <v>93.2</v>
       </c>
@@ -10670,14 +12200,21 @@
       <c r="D74" s="25">
         <v>0.56957841358399997</v>
       </c>
-      <c r="E74" s="17"/>
+      <c r="E74" s="53"/>
       <c r="F74" s="17"/>
       <c r="G74" s="17"/>
       <c r="H74" s="17"/>
       <c r="I74" s="17"/>
       <c r="J74" s="17"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K74" s="17"/>
+      <c r="L74" s="17"/>
+      <c r="M74" s="17"/>
+      <c r="N74" s="17"/>
+      <c r="O74" s="17"/>
+      <c r="P74" s="17"/>
+      <c r="Q74" s="17"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
         <v>94.1</v>
       </c>
@@ -10690,14 +12227,21 @@
       <c r="D75" s="25">
         <v>0.59331624965759999</v>
       </c>
-      <c r="E75" s="17"/>
+      <c r="E75" s="53"/>
       <c r="F75" s="17"/>
       <c r="G75" s="17"/>
       <c r="H75" s="17"/>
       <c r="I75" s="17"/>
       <c r="J75" s="17"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K75" s="17"/>
+      <c r="L75" s="17"/>
+      <c r="M75" s="17"/>
+      <c r="N75" s="17"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
+      <c r="Q75" s="17"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="27">
         <v>95</v>
       </c>
@@ -10710,14 +12254,21 @@
       <c r="D76" s="25">
         <v>0.6221741633408</v>
       </c>
-      <c r="E76" s="17"/>
+      <c r="E76" s="53"/>
       <c r="F76" s="17"/>
       <c r="G76" s="17"/>
       <c r="H76" s="17"/>
       <c r="I76" s="17"/>
       <c r="J76" s="17"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K76" s="17"/>
+      <c r="L76" s="17"/>
+      <c r="M76" s="17"/>
+      <c r="N76" s="17"/>
+      <c r="O76" s="17"/>
+      <c r="P76" s="17"/>
+      <c r="Q76" s="17"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="27">
         <v>95.9</v>
       </c>
@@ -10730,14 +12281,21 @@
       <c r="D77" s="25">
         <v>0.66003374539039994</v>
       </c>
-      <c r="E77" s="17"/>
+      <c r="E77" s="53"/>
       <c r="F77" s="17"/>
       <c r="G77" s="17"/>
       <c r="H77" s="17"/>
       <c r="I77" s="17"/>
       <c r="J77" s="17"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K77" s="17"/>
+      <c r="L77" s="17"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
+      <c r="Q77" s="17"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="27">
         <v>96.8</v>
       </c>
@@ -10750,14 +12308,21 @@
       <c r="D78" s="25">
         <v>0.7195324357888</v>
       </c>
-      <c r="E78" s="17"/>
+      <c r="E78" s="53"/>
       <c r="F78" s="17"/>
       <c r="G78" s="17"/>
       <c r="H78" s="17"/>
       <c r="I78" s="17"/>
       <c r="J78" s="17"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K78" s="17"/>
+      <c r="L78" s="17"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+      <c r="P78" s="17"/>
+      <c r="Q78" s="17"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="28">
         <v>97.47</v>
       </c>
@@ -10770,16 +12335,23 @@
       <c r="D79" s="26">
         <v>0.8770468760672</v>
       </c>
-      <c r="E79" s="18"/>
+      <c r="E79" s="105"/>
       <c r="F79" s="17"/>
       <c r="G79" s="17"/>
       <c r="H79" s="17"/>
       <c r="I79" s="17"/>
-      <c r="J79" s="18"/>
-      <c r="K79" s="51"/>
-      <c r="L79" s="22"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J79" s="17"/>
+      <c r="K79" s="18"/>
+      <c r="L79" s="17"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
+      <c r="Q79" s="18"/>
+      <c r="R79" s="51"/>
+      <c r="S79" s="22"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="27"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
@@ -13000,13 +14572,17 @@
       <c r="A819" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F60:G60"/>
+  <mergeCells count="7">
+    <mergeCell ref="L60:M60"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:H1"/>
+    <mergeCell ref="F60:G60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>